<commit_message>
Cleaning up spreadsheet. Adding GNU license.
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="302">
   <si>
     <t>yr</t>
   </si>
@@ -395,9 +395,6 @@
     <t>maintenance proportion</t>
   </si>
   <si>
-    <t>model y intercept</t>
-  </si>
-  <si>
     <t>model high latitude</t>
   </si>
   <si>
@@ -930,6 +927,12 @@
   </si>
   <si>
     <t>Baseline C</t>
+  </si>
+  <si>
+    <t>model y intercept (==prod_lo)</t>
+  </si>
+  <si>
+    <t>Assumption</t>
   </si>
 </sst>
 </file>
@@ -989,7 +992,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1014,6 +1017,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2593,7 +2608,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2616,15 +2631,22 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1567">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4634,7 +4656,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4665,7 +4687,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="14">
         <f>Settings!G16</f>
@@ -4676,7 +4698,7 @@
         <v>gC gBiomass-1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>118</v>
@@ -4684,7 +4706,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B3" s="14">
         <f>Settings!G17</f>
@@ -4695,7 +4717,7 @@
         <v>gN gBiomass-1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>118</v>
@@ -4703,7 +4725,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" s="14">
         <f>Settings!G18</f>
@@ -4714,7 +4736,7 @@
         <v>gP gBiomass-1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>118</v>
@@ -4722,7 +4744,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5" s="14">
         <f>Settings!B10</f>
@@ -4733,7 +4755,7 @@
         <v>ppm</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>118</v>
@@ -4741,7 +4763,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6" s="14">
         <f>Settings!B12</f>
@@ -4752,7 +4774,7 @@
         <v>ppm yr-1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>118</v>
@@ -4760,7 +4782,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7" s="14">
         <f>Settings!B6</f>
@@ -4771,7 +4793,7 @@
         <v>deg</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>118</v>
@@ -4779,7 +4801,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" s="14">
         <f>Settings!B7</f>
@@ -4790,7 +4812,7 @@
         <v>deg</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>118</v>
@@ -4798,7 +4820,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B9" s="14">
         <f>Settings!B3</f>
@@ -4809,7 +4831,7 @@
         <v>t ha-1 yr-1</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>118</v>
@@ -4817,7 +4839,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B10" s="14">
         <f>Settings!B5</f>
@@ -4828,7 +4850,7 @@
         <v>t ha-1 yr-1</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>118</v>
@@ -4836,7 +4858,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B11" s="14">
         <f>Settings!B8</f>
@@ -4847,7 +4869,7 @@
         <v>t ha-1 yr-1 deg-1</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>118</v>
@@ -4855,18 +4877,18 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B12" s="14">
-        <f>Settings!B5</f>
-        <v>91.3125</v>
+        <f>Settings!B9</f>
+        <v>91</v>
       </c>
       <c r="C12" s="14" t="str">
         <f>Settings!C5</f>
         <v>t ha-1 yr-1</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>122</v>
+        <v>300</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>118</v>
@@ -4874,7 +4896,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B13" s="14">
         <f>Settings!B18</f>
@@ -4885,7 +4907,7 @@
         <v>Pg yr-1</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>118</v>
@@ -4893,7 +4915,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B14" s="14">
         <f>Settings!B20</f>
@@ -4904,7 +4926,7 @@
         <v>Pg yr-1</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>118</v>
@@ -4912,7 +4934,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B15" s="14">
         <f>Settings!B24</f>
@@ -4931,7 +4953,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B16" s="14">
         <f>Settings!B25</f>
@@ -4950,7 +4972,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B17" s="14">
         <f>Settings!B26</f>
@@ -4969,7 +4991,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B18" s="14">
         <f>Settings!B22</f>
@@ -4980,7 +5002,7 @@
         <v>$ ha-1</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>117</v>
@@ -4988,7 +5010,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" s="14">
         <f>Settings!B23</f>
@@ -4999,7 +5021,7 @@
         <v>$ ha-1</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>117</v>
@@ -5007,7 +5029,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B20" s="14">
         <f>Settings!B27</f>
@@ -5018,7 +5040,7 @@
         <v>$ ha-1 yr-1</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>117</v>
@@ -5026,7 +5048,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B21" s="14">
         <f>Settings!B28</f>
@@ -5037,7 +5059,7 @@
         <v>$ ha-1 yr-1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>117</v>
@@ -5045,7 +5067,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B22" s="14">
         <f>Settings!B29</f>
@@ -5056,7 +5078,7 @@
         <v>yr</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>117</v>
@@ -5064,7 +5086,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B23" s="14">
         <f>Settings!B30</f>
@@ -5075,7 +5097,7 @@
         <v>yr</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>117</v>
@@ -5083,7 +5105,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B24" s="14">
         <f>Settings!B31</f>
@@ -5094,7 +5116,7 @@
         <v>prp</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>117</v>
@@ -5102,7 +5124,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25" s="14">
         <f>Settings!B32</f>
@@ -5113,7 +5135,7 @@
         <v>yr</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>117</v>
@@ -5121,7 +5143,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B26" s="14">
         <f>Settings!B33</f>
@@ -5132,7 +5154,7 @@
         <v>yr</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>117</v>
@@ -5140,7 +5162,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B27" s="14">
         <f>Settings!B34</f>
@@ -5151,7 +5173,7 @@
         <v>yr</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>117</v>
@@ -5190,30 +5212,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="10">
         <v>146.7885378</v>
@@ -5222,18 +5244,18 @@
         <v>-19.257637299999999</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B3" s="10">
         <v>-80.457524599999999</v>
@@ -5242,21 +5264,21 @@
         <v>26.657368099999999</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3">
         <v>2009</v>
       </c>
       <c r="G3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="10">
         <v>-74.539295999999993</v>
@@ -5265,11 +5287,11 @@
         <v>40.372374000000001</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" s="10"/>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5283,16 +5305,16 @@
         <v>37.855311</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" s="10"/>
       <c r="G5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B6" s="10">
         <v>-120.9</v>
@@ -5301,16 +5323,16 @@
         <v>50.8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="10"/>
       <c r="G6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="10">
         <v>-119.7</v>
@@ -5319,11 +5341,11 @@
         <v>50.8</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="10"/>
       <c r="G7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5337,16 +5359,16 @@
         <v>17.45</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E8" s="10"/>
       <c r="G8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="10">
         <v>120.3</v>
@@ -5355,11 +5377,11 @@
         <v>23</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E9" s="10"/>
       <c r="G9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5373,16 +5395,16 @@
         <v>24.520453</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E10" s="10"/>
       <c r="G10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" s="10">
         <v>-121.132778</v>
@@ -5391,16 +5413,16 @@
         <v>37.473056</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5414,11 +5436,11 @@
         <v>27.427821999999999</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="10"/>
       <c r="G12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5432,16 +5454,16 @@
         <v>37.223215000000003</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B14">
         <v>-79.024995599999997</v>
@@ -5450,21 +5472,21 @@
         <v>36.001745499999998</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" t="s">
         <v>163</v>
       </c>
-      <c r="F14" t="s">
-        <v>164</v>
-      </c>
       <c r="G14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="10">
         <v>-80.907136899999998</v>
@@ -5473,21 +5495,21 @@
         <v>27.213987700000001</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16">
         <v>-81.965361400000006</v>
@@ -5496,15 +5518,15 @@
         <v>27.8745254</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B17" s="10">
         <v>-81.880556400000003</v>
@@ -5513,21 +5535,21 @@
         <v>26.674672000000001</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F17">
         <v>2009</v>
       </c>
       <c r="G17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18" s="10">
         <v>-80.853750700000006</v>
@@ -5536,21 +5558,21 @@
         <v>27.329125999999999</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B19">
         <v>-80.869715799999994</v>
@@ -5559,21 +5581,21 @@
         <v>27.5020904</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20">
         <v>-80.398945299999994</v>
@@ -5582,21 +5604,21 @@
         <v>27.592262000000002</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21">
         <v>-80.399409399999996</v>
@@ -5605,21 +5627,21 @@
         <v>27.602654600000001</v>
       </c>
       <c r="D21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="F21">
         <v>2010</v>
       </c>
       <c r="G21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B22" s="10">
         <v>-80.479466200000005</v>
@@ -5628,21 +5650,21 @@
         <v>27.609477500000001</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B23" s="10">
         <v>-81.445307999999997</v>
@@ -5651,21 +5673,21 @@
         <v>28.5647631</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F23">
         <v>2009</v>
       </c>
       <c r="G23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B24" s="10">
         <v>-82.477197000000004</v>
@@ -5674,21 +5696,21 @@
         <v>29.923072999999999</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B25" s="10">
         <v>-85.024425500000007</v>
@@ -5697,21 +5719,21 @@
         <v>34.827157800000002</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B26">
         <v>-76.535835800000001</v>
@@ -5720,21 +5742,21 @@
         <v>39.197844400000001</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" t="s">
         <v>161</v>
       </c>
-      <c r="F26" t="s">
-        <v>162</v>
-      </c>
       <c r="G26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B27">
         <v>-76.519799699999993</v>
@@ -5743,21 +5765,21 @@
         <v>39.241779600000001</v>
       </c>
       <c r="D27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F27">
         <v>2015</v>
       </c>
       <c r="G27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B28">
         <v>-76.262986100000006</v>
@@ -5766,21 +5788,21 @@
         <v>39.7560024</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F28">
         <v>2009</v>
       </c>
       <c r="G28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B29" s="10">
         <v>-73.828925999999996</v>
@@ -5789,21 +5811,21 @@
         <v>40.584173399999997</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B30" s="10">
         <v>3.5740601999999999</v>
@@ -5812,16 +5834,16 @@
         <v>51.082552</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E30" s="10"/>
       <c r="G30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B31" s="10">
         <v>16.430962999999998</v>
@@ -5830,11 +5852,11 @@
         <v>48.197578999999998</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5848,12 +5870,12 @@
         <v>-19.3</v>
       </c>
       <c r="G32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B33" s="10">
         <v>-76.900000000000006</v>
@@ -5862,11 +5884,11 @@
         <v>39</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E33" s="10"/>
       <c r="G33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5880,11 +5902,11 @@
         <v>38.784427000000001</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E34" s="10"/>
       <c r="G34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5898,10 +5920,10 @@
         <v>39.131529</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5915,10 +5937,10 @@
         <v>39.449888999999999</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5932,11 +5954,11 @@
         <v>38.609043200000002</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E37" s="10"/>
       <c r="G37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5950,16 +5972,16 @@
         <v>37.247632000000003</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5973,16 +5995,16 @@
         <v>36.200000000000003</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F39">
         <v>2009</v>
       </c>
       <c r="G39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5996,16 +6018,16 @@
         <v>36.080810999999997</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -6019,16 +6041,16 @@
         <v>29.645575999999998</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E41" s="10"/>
       <c r="G41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B42" s="10">
         <v>-98.806156999999999</v>
@@ -6037,21 +6059,21 @@
         <v>29.491195399999999</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B43" s="10">
         <v>16.163287777777775</v>
@@ -6060,16 +6082,16 @@
         <v>51.627626666666664</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" s="10"/>
       <c r="G43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B44">
         <v>-103.3499748</v>
@@ -6078,21 +6100,21 @@
         <v>34.178595899999998</v>
       </c>
       <c r="D44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45" s="10">
         <v>-75.900000000000006</v>
@@ -6101,11 +6123,11 @@
         <v>39</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E45" s="10"/>
       <c r="G45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6135,8 +6157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:D36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6160,80 +6182,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="A1" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="F1" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="13">
+      <c r="A2" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="21">
         <v>15</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="D2" s="20"/>
+      <c r="F2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="21">
         <v>365.25</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="12" t="str">
+      <c r="A3" s="20" t="str">
         <f>A2</f>
         <v>ATS productivity (high lat)</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="21">
         <f>B2*$G$2*$G$3/$G$4</f>
         <v>54.787500000000001</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="D3" s="20"/>
+      <c r="F3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="21">
         <f>100*100</f>
         <v>10000</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="20" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="13">
+      <c r="A4" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="21">
         <v>25</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="D4" s="20"/>
+      <c r="F4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="21">
         <v>1000000</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -6249,19 +6274,20 @@
       <c r="C5" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="12"/>
+      <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="14">
         <v>1000</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B6" s="13">
         <v>40</v>
@@ -6269,19 +6295,20 @@
       <c r="C6" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F6" t="s">
-        <v>203</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="D6" s="12"/>
+      <c r="F6" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G6" s="14">
         <v>1000</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -6289,6 +6316,7 @@
       <c r="C7" s="12" t="s">
         <v>96</v>
       </c>
+      <c r="D7" s="12"/>
       <c r="F7" t="s">
         <v>13</v>
       </c>
@@ -6301,7 +6329,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B8" s="13">
         <f>(B5-B3)/(B7-B6)</f>
@@ -6310,6 +6338,7 @@
       <c r="C8" s="12" t="s">
         <v>100</v>
       </c>
+      <c r="D8" s="12"/>
       <c r="F8" t="s">
         <v>14</v>
       </c>
@@ -6322,7 +6351,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B9" s="13">
         <v>91</v>
@@ -6330,6 +6359,7 @@
       <c r="C9" s="12" t="s">
         <v>102</v>
       </c>
+      <c r="D9" s="12"/>
       <c r="F9" t="s">
         <v>101</v>
       </c>
@@ -6343,7 +6373,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B10" s="13">
         <v>410</v>
@@ -6351,8 +6381,9 @@
       <c r="C10" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="D10" s="12"/>
       <c r="F10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G10" s="1">
         <v>1000</v>
@@ -6362,17 +6393,17 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B11" s="13">
+      <c r="A11" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="B11" s="21">
         <f>B10*G32</f>
         <v>873300000000</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="21"/>
       <c r="F11" t="s">
         <v>11</v>
       </c>
@@ -6386,7 +6417,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B12" s="13">
         <v>2</v>
@@ -6394,8 +6425,8 @@
       <c r="C12" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D12" t="s">
-        <v>289</v>
+      <c r="D12" s="12" t="s">
+        <v>288</v>
       </c>
       <c r="F12" t="s">
         <v>70</v>
@@ -6409,16 +6440,17 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="B13" s="13">
+      <c r="A13" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="21">
         <f>B12*G32</f>
         <v>4260000000</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="20" t="s">
         <v>103</v>
       </c>
+      <c r="D13" s="20"/>
       <c r="F13" t="s">
         <v>71</v>
       </c>
@@ -6443,13 +6475,13 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="16" t="s">
-        <v>293</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="A15" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F15" t="s">
         <v>72</v>
@@ -6463,14 +6495,17 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B16" s="14">
+      <c r="A16" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="23">
         <v>5</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="22" t="s">
         <v>2</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>301</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>115</v>
@@ -6506,7 +6541,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18" s="13">
         <v>104.9</v>
@@ -6515,7 +6550,7 @@
         <v>104</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>115</v>
@@ -6529,30 +6564,31 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" t="s">
-        <v>202</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="A19" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="14">
         <f>B18*$G$8/$G$6</f>
         <v>104900000000000</v>
       </c>
-      <c r="C19" t="s">
-        <v>204</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="C19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="F19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="14">
         <v>0.26417200000000002</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B20" s="13">
         <v>8</v>
@@ -6561,38 +6597,39 @@
         <v>104</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="F20" t="s">
+        <v>297</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="14">
         <v>2.47105</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="1">
+      <c r="A21" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" s="14">
         <f>B20*$G$8/$G$6</f>
         <v>8000000000000</v>
       </c>
-      <c r="C21" t="s">
-        <v>204</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="C21" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="F21" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="14">
         <f>1/2.54</f>
         <v>0.39370078740157477</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="5" t="s">
         <v>92</v>
       </c>
     </row>
@@ -6606,16 +6643,16 @@
       <c r="C22" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D22" t="s">
-        <v>273</v>
-      </c>
-      <c r="F22" t="s">
-        <v>196</v>
-      </c>
-      <c r="G22" s="1">
+      <c r="D22" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G22" s="14">
         <v>3.28084</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="14" t="s">
         <v>16</v>
       </c>
       <c r="K22" s="1"/>
@@ -6630,17 +6667,17 @@
       <c r="C23" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D23" t="s">
-        <v>273</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="D23" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G23" s="14">
+        <v>1.3079499999999999</v>
+      </c>
+      <c r="H23" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1.3079499999999999</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="K23" s="1"/>
     </row>
@@ -6654,18 +6691,18 @@
       <c r="C24" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D24" t="s">
-        <v>273</v>
+      <c r="D24" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" t="s">
+      <c r="F24" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="14">
         <f>1000000*G25/2000</f>
         <v>1.1023099999999999</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="14" t="s">
         <v>94</v>
       </c>
       <c r="K24" s="1"/>
@@ -6680,17 +6717,17 @@
       <c r="C25" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D25" t="s">
-        <v>273</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="D25" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="14">
         <f>0.00220462</f>
         <v>2.20462E-3</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6704,16 +6741,16 @@
       <c r="C26" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="D26" t="s">
-        <v>273</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="D26" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="14">
         <v>9.2902999999999998E-6</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -6728,13 +6765,14 @@
       <c r="C27" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="F27" t="s">
+      <c r="D27" s="12"/>
+      <c r="F27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="14">
         <v>5280</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -6749,19 +6787,20 @@
       <c r="C28" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="D28" s="12"/>
+      <c r="F28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="14">
         <v>0.453592</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="H28" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B29" s="13">
         <v>40</v>
@@ -6769,23 +6808,23 @@
       <c r="C29" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D29" t="s">
-        <v>273</v>
-      </c>
-      <c r="F29" s="12" t="s">
+      <c r="D29" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G29" s="13">
+      <c r="G29" s="14">
         <v>6.4515999999999998E-4</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="5" t="s">
         <v>105</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B30" s="13">
         <v>20</v>
@@ -6793,17 +6832,17 @@
       <c r="C30" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D30" t="s">
-        <v>273</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="D30" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="5">
         <v>1.60934</v>
       </c>
-      <c r="H30" t="s">
-        <v>278</v>
+      <c r="H30" s="5" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -6814,24 +6853,24 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D31" t="s">
-        <v>273</v>
-      </c>
-      <c r="F31" t="s">
-        <v>278</v>
-      </c>
-      <c r="G31" s="1">
+        <v>210</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G31" s="14">
         <v>1000</v>
       </c>
-      <c r="H31" t="s">
-        <v>196</v>
+      <c r="H31" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B32" s="13">
         <v>50</v>
@@ -6839,22 +6878,22 @@
       <c r="C32" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D32" t="s">
-        <v>273</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="D32" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="G32" s="21">
         <v>2130000000</v>
       </c>
-      <c r="H32" s="12" t="s">
-        <v>290</v>
+      <c r="H32" s="20" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B33" s="13">
         <v>100</v>
@@ -6862,13 +6901,16 @@
       <c r="C33" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D33" t="s">
-        <v>273</v>
-      </c>
+      <c r="D33" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B34" s="13">
         <v>200</v>
@@ -6876,61 +6918,70 @@
       <c r="C34" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D34" t="s">
-        <v>273</v>
-      </c>
+      <c r="D34" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" t="s">
+      <c r="A37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" t="s">
+      <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="14">
         <v>106</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="14">
         <f>G12*B38</f>
         <v>1273.1659999999999</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="14">
         <f>C38/C$41</f>
         <v>0.83308860865513967</v>
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" t="s">
+      <c r="A39" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="14">
         <v>16</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="14">
         <f>G13*B39</f>
         <v>224.11199999999999</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="14">
         <f>C39/C$41</f>
         <v>0.1466463558270647</v>
       </c>
@@ -7028,10 +7079,10 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
@@ -7074,10 +7125,10 @@
         <v>22</v>
       </c>
       <c r="R2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -7126,7 +7177,7 @@
         <v>27</v>
       </c>
       <c r="R3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="S3" s="1">
         <v>53.4</v>
@@ -7181,11 +7232,11 @@
         <v>28</v>
       </c>
       <c r="R4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S4" s="1">
         <f>'R Variables'!$B$11*Wetlands!S3+'R Variables'!$B$12</f>
-        <v>42.551625000000001</v>
+        <v>42.239125000000001</v>
       </c>
       <c r="T4" t="s">
         <v>102</v>
@@ -7280,7 +7331,7 @@
         <v>0.35</v>
       </c>
       <c r="T6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -7363,7 +7414,7 @@
         <v>3785.41</v>
       </c>
       <c r="R8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S8" s="1">
         <v>0.4</v>
@@ -7415,7 +7466,7 @@
         <v>0.26</v>
       </c>
       <c r="T9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -7482,7 +7533,7 @@
       </c>
       <c r="L11" s="2"/>
       <c r="R11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="S11" s="1">
         <f>S7/Settings!G17</f>
@@ -7494,7 +7545,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="R12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S12" s="1">
         <f>S10/Settings!$G$18</f>
@@ -7515,47 +7566,47 @@
       </c>
       <c r="L13" s="2"/>
       <c r="R13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="S13" s="1">
         <f>$S$4/S11</f>
-        <v>2.084161224489796</v>
+        <v>2.0688551020408168</v>
       </c>
       <c r="T13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="R14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S14" s="1">
         <f>$S$4/S12</f>
-        <v>1.2274507211538461</v>
+        <v>1.218436298076923</v>
       </c>
       <c r="T14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="R16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="18:20">
       <c r="R17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="18:20">
       <c r="R18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="S18" s="1">
         <v>7.3</v>
@@ -7566,11 +7617,11 @@
     </row>
     <row r="19" spans="18:20">
       <c r="R19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S19" s="1">
         <f>'R Variables'!$B$11*Wetlands!S18+'R Variables'!$B$12</f>
-        <v>84.646687499999999</v>
+        <v>84.334187499999999</v>
       </c>
       <c r="T19" t="s">
         <v>102</v>
@@ -7578,7 +7629,7 @@
     </row>
     <row r="20" spans="18:20">
       <c r="R20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S20" s="1">
         <v>25</v>
@@ -7589,7 +7640,7 @@
     </row>
     <row r="21" spans="18:20">
       <c r="R21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S21" s="1">
         <f>S20/Settings!G3</f>
@@ -7601,48 +7652,48 @@
     </row>
     <row r="22" spans="18:20">
       <c r="R22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S22" s="1">
         <v>13</v>
       </c>
       <c r="T22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="18:20">
       <c r="R23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S23" s="1">
         <f>S22*Settings!$G$10</f>
         <v>13000</v>
       </c>
       <c r="T23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="18:20">
       <c r="R24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S24" s="1">
         <v>1.36</v>
       </c>
       <c r="T24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="18:20">
       <c r="R25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S25" s="1">
         <f>S24*$S$23</f>
         <v>17680</v>
       </c>
       <c r="T25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="18:20">
@@ -7653,7 +7704,7 @@
         <v>0.19</v>
       </c>
       <c r="T26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="18:20">
@@ -7665,7 +7716,7 @@
         <v>3359.2</v>
       </c>
       <c r="T27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="18:20">
@@ -7677,7 +7728,7 @@
         <v>1226947.8</v>
       </c>
       <c r="T28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="18:20">
@@ -7706,7 +7757,7 @@
     </row>
     <row r="31" spans="18:20">
       <c r="R31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S31" s="1" t="e">
         <f>S30/Settings!$G$18</f>
@@ -7718,23 +7769,23 @@
     </row>
     <row r="33" spans="18:20">
       <c r="R33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="18:20">
       <c r="R34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="18:20">
       <c r="R35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="S35" s="1">
         <v>24.8</v>
@@ -7745,11 +7796,11 @@
     </row>
     <row r="36" spans="18:20">
       <c r="R36" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S36" s="1">
         <f>'R Variables'!$B$11*Wetlands!S35+'R Variables'!$B$12</f>
-        <v>68.667000000000002</v>
+        <v>68.354500000000002</v>
       </c>
       <c r="T36" t="s">
         <v>102</v>
@@ -7757,7 +7808,7 @@
     </row>
     <row r="37" spans="18:20">
       <c r="R37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S37" s="1">
         <v>1.07</v>
@@ -7768,48 +7819,48 @@
     </row>
     <row r="38" spans="18:20">
       <c r="R38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S38" s="1">
         <v>4000</v>
       </c>
       <c r="T38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="18:20">
       <c r="R39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="S39" s="1">
         <f>S38*Settings!$G$10</f>
         <v>4000000</v>
       </c>
       <c r="T39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="18:20">
       <c r="R40" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S40" s="1">
         <v>1.9</v>
       </c>
       <c r="T40" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="18:20">
       <c r="R41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S41" s="1">
         <f>S40*$S$23</f>
         <v>24700</v>
       </c>
       <c r="T41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="18:20">
@@ -7820,7 +7871,7 @@
         <v>0.44</v>
       </c>
       <c r="T42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="18:20">
@@ -7832,7 +7883,7 @@
         <v>10868</v>
       </c>
       <c r="T43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="18:20">
@@ -7844,7 +7895,7 @@
         <v>3969537</v>
       </c>
       <c r="T44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="45" spans="18:20">
@@ -7873,7 +7924,7 @@
     </row>
     <row r="47" spans="18:20">
       <c r="R47" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S47" s="1" t="e">
         <f>S46/Settings!$G$18</f>
@@ -7920,7 +7971,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>63</v>
@@ -7929,12 +7980,12 @@
         <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" s="1">
         <f>[1]A!$R$66</f>
@@ -7944,24 +7995,24 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" s="1">
         <f>'Highway Costs'!B2*Settings!G31*Settings!G30</f>
         <v>14107553603.434601</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -7970,24 +8021,24 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B5" s="1">
         <f>B4/Settings!G22</f>
         <v>3.6575998829568039</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B6" s="1">
         <f>B5*B3</f>
@@ -7999,7 +8050,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B7" s="1">
         <f>B6/Settings!G3</f>
@@ -8011,7 +8062,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B8" s="1">
         <f>1000*[2]HF2!$E$67</f>
@@ -8021,12 +8072,12 @@
         <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B9" s="1">
         <f>1000*[2]HF2!$I$67</f>
@@ -8036,12 +8087,12 @@
         <v>95</v>
       </c>
       <c r="D9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B10" s="1">
         <f>B9+B8</f>
@@ -8053,14 +8104,14 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B11" s="1">
         <f>B10/B7</f>
         <v>30400.509579137084</v>
       </c>
       <c r="C11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:4">

</xml_diff>

<commit_message>
Getting rid of NP sums.
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="311">
   <si>
     <t>yr</t>
   </si>
@@ -377,27 +377,12 @@
     <t>ecol</t>
   </si>
   <si>
-    <t>hectares per employee</t>
-  </si>
-  <si>
-    <t>employee salary</t>
-  </si>
-  <si>
-    <t>maintenance proportion</t>
-  </si>
-  <si>
     <t>model high latitude</t>
   </si>
   <si>
     <t>model slope</t>
   </si>
   <si>
-    <t>high OPEX</t>
-  </si>
-  <si>
-    <t>low OPEX</t>
-  </si>
-  <si>
     <t>C:biomass ratio</t>
   </si>
   <si>
@@ -407,12 +392,6 @@
     <t>P:biomass ratio</t>
   </si>
   <si>
-    <t>low CAPEX</t>
-  </si>
-  <si>
-    <t>high CAPEX</t>
-  </si>
-  <si>
     <t>Growth rate, atmospheric CO2</t>
   </si>
   <si>
@@ -629,9 +608,6 @@
     <t>Kg</t>
   </si>
   <si>
-    <t>Kg yr-1</t>
-  </si>
-  <si>
     <t>Ag NPP</t>
   </si>
   <si>
@@ -951,6 +927,39 @@
   </si>
   <si>
     <t>lbP lbBiomass-1</t>
+  </si>
+  <si>
+    <t>T yr-1</t>
+  </si>
+  <si>
+    <t>ac emp-1</t>
+  </si>
+  <si>
+    <t>employee salary, fully encumbered</t>
+  </si>
+  <si>
+    <t>area per employee</t>
+  </si>
+  <si>
+    <t>maintenance proportion, estimated</t>
+  </si>
+  <si>
+    <t>low CapEx</t>
+  </si>
+  <si>
+    <t>high CapEx</t>
+  </si>
+  <si>
+    <t>low OpEx</t>
+  </si>
+  <si>
+    <t>high OpEx</t>
+  </si>
+  <si>
+    <t>$ ac-1</t>
+  </si>
+  <si>
+    <t>$ ac-1 yr-1</t>
   </si>
 </sst>
 </file>
@@ -1063,8 +1072,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1589">
+  <cellStyleXfs count="1605">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2696,7 +2721,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1589">
+  <cellStyles count="1605">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3491,6 +3516,14 @@
     <cellStyle name="Followed Hyperlink" xfId="1584" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1586" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1604" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4285,6 +4318,14 @@
     <cellStyle name="Hyperlink" xfId="1583" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1585" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1603" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4725,8 +4766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4736,7 +4777,7 @@
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4751,10 +4792,10 @@
         <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>108</v>
@@ -4765,7 +4806,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B2" s="14">
         <f>Settings!G13</f>
@@ -4780,10 +4821,10 @@
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>115</v>
@@ -4791,7 +4832,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B3" s="14">
         <f>Settings!G14</f>
@@ -4806,10 +4847,10 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>115</v>
@@ -4817,7 +4858,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B4" s="14">
         <f>Settings!G15</f>
@@ -4832,10 +4873,10 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>115</v>
@@ -4843,7 +4884,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B5" s="14">
         <f>Settings!B10</f>
@@ -4853,16 +4894,10 @@
         <f>Settings!C10</f>
         <v>ppm</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>410</v>
-      </c>
-      <c r="E5" s="1" t="str">
-        <f>C5</f>
-        <v>ppm</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>115</v>
@@ -4870,7 +4905,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B6" s="14">
         <f>Settings!B12</f>
@@ -4880,16 +4915,10 @@
         <f>Settings!C12</f>
         <v>ppm yr-1</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="str">
-        <f t="shared" ref="E6:E8" si="1">C6</f>
-        <v>ppm yr-1</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>115</v>
@@ -4897,7 +4926,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B7" s="14">
         <f>Settings!B6</f>
@@ -4907,16 +4936,10 @@
         <f>Settings!C6</f>
         <v>deg</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="E7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>deg</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>115</v>
@@ -4924,7 +4947,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B8" s="14">
         <f>Settings!B7</f>
@@ -4934,16 +4957,10 @@
         <f>Settings!C7</f>
         <v>deg</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>deg</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>115</v>
@@ -4951,7 +4968,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B9" s="14">
         <f>Settings!B3</f>
@@ -4966,10 +4983,10 @@
         <v>24.440189478322718</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>115</v>
@@ -4977,7 +4994,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B10" s="14">
         <f>Settings!B5</f>
@@ -4992,10 +5009,10 @@
         <v>40.733649130537863</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>115</v>
@@ -5003,7 +5020,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B11" s="14">
         <f>Settings!B8</f>
@@ -5018,10 +5035,10 @@
         <v>-0.40733649130537863</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>115</v>
@@ -5029,7 +5046,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B12" s="14">
         <f>Settings!B9</f>
@@ -5044,10 +5061,10 @@
         <v>40.594245813869357</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>115</v>
@@ -5055,18 +5072,25 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B13" s="14">
-        <f>Settings!B18</f>
-        <v>104.9</v>
+        <f>Settings!B19</f>
+        <v>104900000000</v>
       </c>
       <c r="C13" s="14" t="str">
-        <f>Settings!C18</f>
-        <v>Pg yr-1</v>
+        <f>Settings!C19</f>
+        <v>t yr-1</v>
+      </c>
+      <c r="D13" s="1">
+        <f>B13*Settings!$G$32*Settings!$G$18</f>
+        <v>46794905339.284569</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>115</v>
@@ -5074,18 +5098,25 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B14" s="14">
-        <f>Settings!B20</f>
-        <v>8</v>
+        <f>Settings!B21</f>
+        <v>8000000000</v>
       </c>
       <c r="C14" s="14" t="str">
-        <f>Settings!C20</f>
-        <v>Pg yr-1</v>
+        <f>Settings!C21</f>
+        <v>t yr-1</v>
+      </c>
+      <c r="D14" s="1">
+        <f>B14*Settings!$G$32*Settings!$G$18</f>
+        <v>3568724906.7137895</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>300</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>115</v>
@@ -5093,7 +5124,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B15" s="14">
         <f>Settings!B24</f>
@@ -5103,8 +5134,15 @@
         <f>Settings!C24</f>
         <v>ha emp-1</v>
       </c>
+      <c r="D15" s="1">
+        <f>B15*Settings!G17</f>
+        <v>12.35525</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>301</v>
+      </c>
       <c r="F15" s="5" t="s">
-        <v>116</v>
+        <v>303</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>114</v>
@@ -5112,7 +5150,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B16" s="14">
         <f>Settings!B25</f>
@@ -5123,7 +5161,7 @@
         <v>$ yr-1</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>117</v>
+        <v>302</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>114</v>
@@ -5131,7 +5169,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B17" s="14">
         <f>Settings!B26</f>
@@ -5142,7 +5180,7 @@
         <v>opex yr-1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>118</v>
+        <v>304</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>114</v>
@@ -5150,7 +5188,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B18" s="14">
         <f>Settings!B22</f>
@@ -5160,8 +5198,15 @@
         <f>Settings!C22</f>
         <v>$ ha-1</v>
       </c>
+      <c r="D18" s="1">
+        <f>B18/Settings!G$17</f>
+        <v>101171.56674288258</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="F18" s="5" t="s">
-        <v>126</v>
+        <v>305</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>114</v>
@@ -5169,7 +5214,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B19" s="14">
         <f>Settings!B23</f>
@@ -5179,8 +5224,15 @@
         <f>Settings!C23</f>
         <v>$ ha-1</v>
       </c>
+      <c r="D19" s="1">
+        <f>B19/Settings!G$17</f>
+        <v>404686.26697153033</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="F19" s="5" t="s">
-        <v>127</v>
+        <v>306</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>114</v>
@@ -5188,7 +5240,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B20" s="14">
         <f>Settings!B27</f>
@@ -5198,8 +5250,15 @@
         <f>Settings!C27</f>
         <v>$ ha-1 yr-1</v>
       </c>
+      <c r="D20" s="1">
+        <f>B20/Settings!G$17</f>
+        <v>13152.303676574735</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="F20" s="5" t="s">
-        <v>122</v>
+        <v>307</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>114</v>
@@ -5207,7 +5266,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B21" s="14">
         <f>Settings!B28</f>
@@ -5217,8 +5276,15 @@
         <f>Settings!C28</f>
         <v>$ ha-1 yr-1</v>
       </c>
+      <c r="D21" s="1">
+        <f>B21/Settings!G$17</f>
+        <v>28328.038688007124</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="F21" s="5" t="s">
-        <v>121</v>
+        <v>308</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>114</v>
@@ -5226,7 +5292,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B22" s="14">
         <f>Settings!B29</f>
@@ -5237,7 +5303,7 @@
         <v>yr</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>114</v>
@@ -5245,7 +5311,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B23" s="14">
         <f>Settings!B30</f>
@@ -5256,7 +5322,7 @@
         <v>yr</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>114</v>
@@ -5264,7 +5330,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B24" s="14">
         <f>Settings!B31</f>
@@ -5275,7 +5341,7 @@
         <v>prp</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>114</v>
@@ -5283,7 +5349,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B25" s="14">
         <f>Settings!B32</f>
@@ -5294,7 +5360,7 @@
         <v>yr</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>114</v>
@@ -5302,7 +5368,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B26" s="14">
         <f>Settings!B33</f>
@@ -5313,7 +5379,7 @@
         <v>yr</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>114</v>
@@ -5321,7 +5387,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B27" s="14">
         <f>Settings!B34</f>
@@ -5332,7 +5398,7 @@
         <v>yr</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>114</v>
@@ -5371,30 +5437,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B2" s="10">
         <v>146.7885378</v>
@@ -5403,18 +5469,18 @@
         <v>-19.257637299999999</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="G2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="10" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B3" s="10">
         <v>-80.457524599999999</v>
@@ -5423,21 +5489,21 @@
         <v>26.657368099999999</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F3">
         <v>2009</v>
       </c>
       <c r="G3" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B4" s="10">
         <v>-74.539295999999993</v>
@@ -5446,11 +5512,11 @@
         <v>40.372374000000001</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E4" s="10"/>
       <c r="G4" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5464,16 +5530,16 @@
         <v>37.855311</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E5" s="10"/>
       <c r="G5" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B6" s="10">
         <v>-120.9</v>
@@ -5482,16 +5548,16 @@
         <v>50.8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E6" s="10"/>
       <c r="G6" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B7" s="10">
         <v>-119.7</v>
@@ -5500,11 +5566,11 @@
         <v>50.8</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E7" s="10"/>
       <c r="G7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5518,16 +5584,16 @@
         <v>17.45</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E8" s="10"/>
       <c r="G8" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B9" s="10">
         <v>120.3</v>
@@ -5536,11 +5602,11 @@
         <v>23</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E9" s="10"/>
       <c r="G9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5554,16 +5620,16 @@
         <v>24.520453</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E10" s="10"/>
       <c r="G10" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B11" s="10">
         <v>-121.132778</v>
@@ -5572,16 +5638,16 @@
         <v>37.473056</v>
       </c>
       <c r="D11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>138</v>
-      </c>
       <c r="F11" s="10" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G11" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5595,11 +5661,11 @@
         <v>27.427821999999999</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E12" s="10"/>
       <c r="G12" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5613,16 +5679,16 @@
         <v>37.223215000000003</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B14">
         <v>-79.024995599999997</v>
@@ -5631,21 +5697,21 @@
         <v>36.001745499999998</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F14" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="G14" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B15" s="10">
         <v>-80.907136899999998</v>
@@ -5654,21 +5720,21 @@
         <v>27.213987700000001</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G15" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B16">
         <v>-81.965361400000006</v>
@@ -5677,15 +5743,15 @@
         <v>27.8745254</v>
       </c>
       <c r="E16" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B17" s="10">
         <v>-81.880556400000003</v>
@@ -5694,21 +5760,21 @@
         <v>26.674672000000001</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F17">
         <v>2009</v>
       </c>
       <c r="G17" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B18" s="10">
         <v>-80.853750700000006</v>
@@ -5717,21 +5783,21 @@
         <v>27.329125999999999</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B19">
         <v>-80.869715799999994</v>
@@ -5740,21 +5806,21 @@
         <v>27.5020904</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G19" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B20">
         <v>-80.398945299999994</v>
@@ -5763,21 +5829,21 @@
         <v>27.592262000000002</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F20" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G20" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B21">
         <v>-80.399409399999996</v>
@@ -5786,21 +5852,21 @@
         <v>27.602654600000001</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F21">
         <v>2010</v>
       </c>
       <c r="G21" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B22" s="10">
         <v>-80.479466200000005</v>
@@ -5809,21 +5875,21 @@
         <v>27.609477500000001</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G22" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B23" s="10">
         <v>-81.445307999999997</v>
@@ -5832,21 +5898,21 @@
         <v>28.5647631</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F23">
         <v>2009</v>
       </c>
       <c r="G23" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B24" s="10">
         <v>-82.477197000000004</v>
@@ -5855,21 +5921,21 @@
         <v>29.923072999999999</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F24" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G24" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B25" s="10">
         <v>-85.024425500000007</v>
@@ -5878,21 +5944,21 @@
         <v>34.827157800000002</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G25" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B26">
         <v>-76.535835800000001</v>
@@ -5901,21 +5967,21 @@
         <v>39.197844400000001</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G26" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B27">
         <v>-76.519799699999993</v>
@@ -5924,21 +5990,21 @@
         <v>39.241779600000001</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F27">
         <v>2015</v>
       </c>
       <c r="G27" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B28">
         <v>-76.262986100000006</v>
@@ -5947,21 +6013,21 @@
         <v>39.7560024</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F28">
         <v>2009</v>
       </c>
       <c r="G28" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B29" s="10">
         <v>-73.828925999999996</v>
@@ -5970,21 +6036,21 @@
         <v>40.584173399999997</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G29" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B30" s="10">
         <v>3.5740601999999999</v>
@@ -5993,16 +6059,16 @@
         <v>51.082552</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E30" s="10"/>
       <c r="G30" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B31" s="10">
         <v>16.430962999999998</v>
@@ -6011,11 +6077,11 @@
         <v>48.197578999999998</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -6029,12 +6095,12 @@
         <v>-19.3</v>
       </c>
       <c r="G32" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B33" s="10">
         <v>-76.900000000000006</v>
@@ -6043,11 +6109,11 @@
         <v>39</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E33" s="10"/>
       <c r="G33" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -6061,11 +6127,11 @@
         <v>38.784427000000001</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E34" s="10"/>
       <c r="G34" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -6079,10 +6145,10 @@
         <v>39.131529</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G35" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -6096,10 +6162,10 @@
         <v>39.449888999999999</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G36" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -6113,11 +6179,11 @@
         <v>38.609043200000002</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E37" s="10"/>
       <c r="G37" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -6131,16 +6197,16 @@
         <v>37.247632000000003</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G38" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -6154,16 +6220,16 @@
         <v>36.200000000000003</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F39">
         <v>2009</v>
       </c>
       <c r="G39" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -6177,16 +6243,16 @@
         <v>36.080810999999997</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E40" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F40" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G40" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -6200,16 +6266,16 @@
         <v>29.645575999999998</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E41" s="10"/>
       <c r="G41" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B42" s="10">
         <v>-98.806156999999999</v>
@@ -6218,21 +6284,21 @@
         <v>29.491195399999999</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G42" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B43" s="10">
         <v>16.163287777777775</v>
@@ -6241,16 +6307,16 @@
         <v>51.627626666666664</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E43" s="10"/>
       <c r="G43" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B44">
         <v>-103.3499748</v>
@@ -6259,21 +6325,21 @@
         <v>34.178595899999998</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F44" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G44" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B45" s="10">
         <v>-75.900000000000006</v>
@@ -6282,11 +6348,11 @@
         <v>39</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E45" s="10"/>
       <c r="G45" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6316,8 +6382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6342,12 +6408,12 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="23" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="15" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>72</v>
@@ -6357,7 +6423,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="16" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B2" s="17">
         <v>15</v>
@@ -6402,7 +6468,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="16" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B4" s="17">
         <v>25</v>
@@ -6435,7 +6501,7 @@
       </c>
       <c r="D5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G5" s="13">
         <v>1000</v>
@@ -6446,7 +6512,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B6" s="13">
         <v>40</v>
@@ -6467,7 +6533,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
@@ -6477,7 +6543,7 @@
       </c>
       <c r="D7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G7" s="13">
         <v>1000</v>
@@ -6488,7 +6554,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B8" s="13">
         <f>(B5-B3)/(B7-B6)</f>
@@ -6511,7 +6577,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B9" s="13">
         <v>91</v>
@@ -6532,7 +6598,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B10" s="13">
         <v>410</v>
@@ -6553,7 +6619,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="16" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B11" s="17">
         <f>B10*G30</f>
@@ -6575,7 +6641,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B12" s="13">
         <v>2</v>
@@ -6584,7 +6650,7 @@
         <v>105</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>71</v>
@@ -6599,7 +6665,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="16" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B13" s="17">
         <f>B12*G30</f>
@@ -6634,12 +6700,12 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="24" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>112</v>
@@ -6654,7 +6720,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="18" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B16" s="19">
         <v>5</v>
@@ -6663,7 +6729,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>21</v>
@@ -6687,7 +6753,7 @@
         <v>86</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>2</v>
@@ -6702,7 +6768,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B18" s="13">
         <v>104.9</v>
@@ -6711,7 +6777,7 @@
         <v>101</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>22</v>
@@ -6727,14 +6793,14 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="16" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B19" s="17">
-        <f>B18*$G$6/$G$5</f>
-        <v>104900000000000</v>
+        <f>B18*$G$6/$G$4</f>
+        <v>104900000000</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D19" s="16"/>
       <c r="F19" s="5" t="s">
@@ -6751,7 +6817,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="12" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B20" s="13">
         <v>8</v>
@@ -6760,10 +6826,10 @@
         <v>101</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="G20" s="14">
         <v>3.28084</v>
@@ -6775,24 +6841,24 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="16" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B21" s="17">
-        <f>B20*$G$6/$G$5</f>
-        <v>8000000000000</v>
+        <f>B20*$G$6/$G$4</f>
+        <v>8000000000</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D21" s="16"/>
       <c r="F21" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G21" s="14">
         <v>1.3079499999999999</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -6806,7 +6872,7 @@
         <v>87</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>91</v>
@@ -6831,7 +6897,7 @@
         <v>87</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>5</v>
@@ -6856,7 +6922,7 @@
         <v>107</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="5" t="s">
@@ -6881,7 +6947,7 @@
         <v>92</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>14</v>
@@ -6904,7 +6970,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
@@ -6957,12 +7023,12 @@
         <v>1.60934</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="12" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B29" s="13">
         <v>40</v>
@@ -6971,22 +7037,22 @@
         <v>0</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="G29" s="14">
         <v>1000</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="12" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B30" s="13">
         <v>20</v>
@@ -6995,16 +7061,16 @@
         <v>0</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="G30" s="17">
         <v>2130000000</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -7015,10 +7081,10 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>4</v>
@@ -7033,7 +7099,7 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="12" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B32" s="13">
         <v>50</v>
@@ -7042,7 +7108,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>4</v>
@@ -7052,12 +7118,12 @@
         <v>1.1023122100918887</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="12" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B33" s="13">
         <v>100</v>
@@ -7066,12 +7132,12 @@
         <v>0</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="12" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B34" s="13">
         <v>200</v>
@@ -7080,7 +7146,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -7237,10 +7303,10 @@
         <v>21</v>
       </c>
       <c r="R1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
@@ -7283,10 +7349,10 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="S2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -7335,7 +7401,7 @@
         <v>26</v>
       </c>
       <c r="R3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="S3" s="1">
         <v>53.4</v>
@@ -7390,7 +7456,7 @@
         <v>27</v>
       </c>
       <c r="R4" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="S4" s="1">
         <f>'R Variables'!$B$11*Wetlands!S3+'R Variables'!$B$12</f>
@@ -7489,7 +7555,7 @@
         <v>0.35</v>
       </c>
       <c r="T6" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -7572,7 +7638,7 @@
         <v>3785.41</v>
       </c>
       <c r="R8" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="S8" s="1">
         <v>0.4</v>
@@ -7624,7 +7690,7 @@
         <v>0.26</v>
       </c>
       <c r="T9" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -7691,7 +7757,7 @@
       </c>
       <c r="L11" s="2"/>
       <c r="R11" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="S11" s="1">
         <f>S7/Settings!G14</f>
@@ -7703,7 +7769,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="R12" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="S12" s="1">
         <f>S10/Settings!$G$15</f>
@@ -7724,47 +7790,47 @@
       </c>
       <c r="L13" s="2"/>
       <c r="R13" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="S13" s="1">
         <f>$S$4/S11</f>
         <v>2.0688551020408168</v>
       </c>
       <c r="T13" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="R14" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="S14" s="1">
         <f>$S$4/S12</f>
         <v>1.218436298076923</v>
       </c>
       <c r="T14" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="R16" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="18:20">
       <c r="R17" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="18:20">
       <c r="R18" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="S18" s="1">
         <v>7.3</v>
@@ -7775,7 +7841,7 @@
     </row>
     <row r="19" spans="18:20">
       <c r="R19" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="S19" s="1">
         <f>'R Variables'!$B$11*Wetlands!S18+'R Variables'!$B$12</f>
@@ -7787,7 +7853,7 @@
     </row>
     <row r="20" spans="18:20">
       <c r="R20" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="S20" s="1">
         <v>25</v>
@@ -7798,7 +7864,7 @@
     </row>
     <row r="21" spans="18:20">
       <c r="R21" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="S21" s="1">
         <f>S20/Settings!G3</f>
@@ -7810,48 +7876,48 @@
     </row>
     <row r="22" spans="18:20">
       <c r="R22" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="S22" s="1">
         <v>13</v>
       </c>
       <c r="T22" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="18:20">
       <c r="R23" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="S23" s="1">
         <f>S22*Settings!$G$7</f>
         <v>13000</v>
       </c>
       <c r="T23" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="18:20">
       <c r="R24" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="S24" s="1">
         <v>1.36</v>
       </c>
       <c r="T24" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="18:20">
       <c r="R25" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="S25" s="1">
         <f>S24*$S$23</f>
         <v>17680</v>
       </c>
       <c r="T25" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="18:20">
@@ -7862,7 +7928,7 @@
         <v>0.19</v>
       </c>
       <c r="T26" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="18:20">
@@ -7874,7 +7940,7 @@
         <v>3359.2</v>
       </c>
       <c r="T27" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="18:20">
@@ -7886,7 +7952,7 @@
         <v>1226947.8</v>
       </c>
       <c r="T28" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="18:20">
@@ -7915,7 +7981,7 @@
     </row>
     <row r="31" spans="18:20">
       <c r="R31" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="S31" s="1" t="e">
         <f>S30/Settings!$G$15</f>
@@ -7927,23 +7993,23 @@
     </row>
     <row r="33" spans="18:20">
       <c r="R33" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="18:20">
       <c r="R34" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="18:20">
       <c r="R35" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="S35" s="1">
         <v>24.8</v>
@@ -7954,7 +8020,7 @@
     </row>
     <row r="36" spans="18:20">
       <c r="R36" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="S36" s="1">
         <f>'R Variables'!$B$11*Wetlands!S35+'R Variables'!$B$12</f>
@@ -7966,7 +8032,7 @@
     </row>
     <row r="37" spans="18:20">
       <c r="R37" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="S37" s="1">
         <v>1.07</v>
@@ -7977,48 +8043,48 @@
     </row>
     <row r="38" spans="18:20">
       <c r="R38" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="S38" s="1">
         <v>4000</v>
       </c>
       <c r="T38" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="18:20">
       <c r="R39" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="S39" s="1">
         <f>S38*Settings!$G$7</f>
         <v>4000000</v>
       </c>
       <c r="T39" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="18:20">
       <c r="R40" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="S40" s="1">
         <v>1.9</v>
       </c>
       <c r="T40" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="41" spans="18:20">
       <c r="R41" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="S41" s="1">
         <f>S40*$S$23</f>
         <v>24700</v>
       </c>
       <c r="T41" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="18:20">
@@ -8029,7 +8095,7 @@
         <v>0.44</v>
       </c>
       <c r="T42" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="18:20">
@@ -8041,7 +8107,7 @@
         <v>10868</v>
       </c>
       <c r="T43" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="18:20">
@@ -8053,7 +8119,7 @@
         <v>3969537</v>
       </c>
       <c r="T44" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="18:20">
@@ -8082,7 +8148,7 @@
     </row>
     <row r="47" spans="18:20">
       <c r="R47" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="S47" s="1" t="e">
         <f>S46/Settings!$G$15</f>
@@ -8129,7 +8195,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>62</v>
@@ -8138,12 +8204,12 @@
         <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B2" s="1">
         <f>[1]A!$R$66</f>
@@ -8153,24 +8219,24 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B3" s="1">
         <f>'Highway Costs'!B2*Settings!G29*Settings!G28</f>
         <v>14107553603.434601</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -8179,24 +8245,24 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B5" s="1">
         <f>B4/Settings!G20</f>
         <v>3.6575998829568039</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B6" s="1">
         <f>B5*B3</f>
@@ -8208,7 +8274,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B7" s="1">
         <f>B6/Settings!G3</f>
@@ -8220,7 +8286,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B8" s="1">
         <f>1000*[2]HF2!$E$67</f>
@@ -8230,12 +8296,12 @@
         <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B9" s="1">
         <f>1000*[2]HF2!$I$67</f>
@@ -8245,12 +8311,12 @@
         <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B10" s="1">
         <f>B9+B8</f>
@@ -8262,14 +8328,14 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B11" s="1">
         <f>B10/B7</f>
         <v>30400.509579137084</v>
       </c>
       <c r="C11" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:4">

</xml_diff>

<commit_message>
Returning to biomass numbers rather than Redfield ratios.
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764"/>
+    <workbookView xWindow="7240" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764"/>
   </bookViews>
   <sheets>
     <sheet name="R Variables" sheetId="12" r:id="rId1"/>
@@ -1078,8 +1078,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1617">
+  <cellStyleXfs count="1619">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2739,7 +2741,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1617">
+  <cellStyles count="1619">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3548,6 +3550,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1612" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1614" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1618" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4356,6 +4359,7 @@
     <cellStyle name="Hyperlink" xfId="1611" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1613" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1617" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4839,8 +4843,8 @@
         <v>235</v>
       </c>
       <c r="B2" s="14">
-        <f>Settings!G16</f>
-        <v>0.83308860865513967</v>
+        <f>Settings!G13</f>
+        <v>0.5</v>
       </c>
       <c r="C2" s="14" t="str">
         <f>Settings!H13&amp;" "&amp;Settings!F13&amp;"-1"</f>
@@ -4848,7 +4852,7 @@
       </c>
       <c r="D2" s="1">
         <f>B2</f>
-        <v>0.83308860865513967</v>
+        <v>0.5</v>
       </c>
       <c r="E2" t="s">
         <v>297</v>
@@ -4865,8 +4869,8 @@
         <v>236</v>
       </c>
       <c r="B3" s="14">
-        <f>Settings!G17</f>
-        <v>0.1466463558270647</v>
+        <f>Settings!G14</f>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C3" s="14" t="str">
         <f>Settings!H14&amp;" "&amp;Settings!F14&amp;"-1"</f>
@@ -4874,7 +4878,7 @@
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D4" si="0">B3</f>
-        <v>0.1466463558270647</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E3" t="s">
         <v>298</v>
@@ -4891,8 +4895,8 @@
         <v>237</v>
       </c>
       <c r="B4" s="14">
-        <f>Settings!G18</f>
-        <v>2.026503551779554E-2</v>
+        <f>Settings!G15</f>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C4" s="14" t="str">
         <f>Settings!H15&amp;" "&amp;Settings!F15&amp;"-1"</f>
@@ -4900,7 +4904,7 @@
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>2.026503551779554E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E4" t="s">
         <v>299</v>
@@ -6412,8 +6416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView topLeftCell="B23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Cleanup and updating algal biomass stoichiometry.
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764"/>
+    <workbookView xWindow="7240" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R Variables" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="314">
   <si>
     <t>yr</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Redfield Ratios</t>
-  </si>
-  <si>
     <t>Atom</t>
   </si>
   <si>
@@ -962,10 +959,16 @@
     <t>$ ac-1 yr-1</t>
   </si>
   <si>
-    <t>non-Redfield</t>
-  </si>
-  <si>
-    <t>Redfield</t>
+    <t>H</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Biomass Stoichiometry (Ebeling et al., 2006)</t>
+  </si>
+  <si>
+    <t>mol H</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1081,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1619">
+  <cellStyleXfs count="1627">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2741,7 +2752,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1619">
+  <cellStyles count="1627">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3551,6 +3562,10 @@
     <cellStyle name="Followed Hyperlink" xfId="1614" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1616" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1626" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4360,6 +4375,10 @@
     <cellStyle name="Hyperlink" xfId="1613" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1615" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1625" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4800,8 +4819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4817,108 +4836,108 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="D1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" t="s">
         <v>293</v>
       </c>
-      <c r="E1" t="s">
-        <v>294</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B2" s="14">
-        <f>Settings!G13</f>
-        <v>0.5</v>
+        <f>Settings!G14</f>
+        <v>0.35830664911296195</v>
       </c>
       <c r="C2" s="14" t="str">
-        <f>Settings!H13&amp;" "&amp;Settings!F13&amp;"-1"</f>
+        <f>Settings!H14&amp;" "&amp;Settings!F14&amp;"-1"</f>
         <v>gC gBiomass-1</v>
       </c>
       <c r="D2" s="1">
         <f>B2</f>
-        <v>0.5</v>
+        <v>0.35830664911296195</v>
       </c>
       <c r="E2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B3" s="14">
-        <f>Settings!G14</f>
-        <v>4.8000000000000001E-2</v>
+        <f>Settings!G15</f>
+        <v>6.3071759492481047E-2</v>
       </c>
       <c r="C3" s="14" t="str">
-        <f>Settings!H14&amp;" "&amp;Settings!F14&amp;"-1"</f>
+        <f>Settings!H15&amp;" "&amp;Settings!F15&amp;"-1"</f>
         <v>gN gBiomass-1</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D4" si="0">B3</f>
-        <v>4.8000000000000001E-2</v>
+        <v>6.3071759492481047E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" s="14">
-        <f>Settings!G15</f>
-        <v>3.0000000000000001E-3</v>
+        <f>Settings!G16</f>
+        <v>8.7158759525689748E-3</v>
       </c>
       <c r="C4" s="14" t="str">
-        <f>Settings!H15&amp;" "&amp;Settings!F15&amp;"-1"</f>
+        <f>Settings!H16&amp;" "&amp;Settings!F16&amp;"-1"</f>
         <v>gP gBiomass-1</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
+        <v>8.7158759525689748E-3</v>
       </c>
       <c r="E4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B5" s="14">
         <f>Settings!B10</f>
@@ -4931,15 +4950,15 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B6" s="14">
         <f>Settings!B12</f>
@@ -4952,15 +4971,15 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B7" s="14">
         <f>Settings!B6</f>
@@ -4973,15 +4992,15 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B8" s="14">
         <f>Settings!B7</f>
@@ -4994,15 +5013,15 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B9" s="14">
         <f>Settings!B3</f>
@@ -5013,22 +5032,22 @@
         <v>t ha-1 yr-1</v>
       </c>
       <c r="D9" s="1">
-        <f>B9*Settings!$G$35*Settings!$G$21</f>
+        <f>B9*Settings!$G$33*Settings!$G$19</f>
         <v>24.440189478322718</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B10" s="14">
         <f>Settings!B5</f>
@@ -5039,22 +5058,22 @@
         <v>t ha-1 yr-1</v>
       </c>
       <c r="D10" s="1">
-        <f>B10*Settings!$G$35*Settings!$G$21</f>
+        <f>B10*Settings!$G$33*Settings!$G$19</f>
         <v>40.733649130537863</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B11" s="14">
         <f>Settings!B8</f>
@@ -5065,22 +5084,22 @@
         <v>t ha-1 yr-1 deg-1</v>
       </c>
       <c r="D11" s="1">
-        <f>B11*Settings!$G$35*Settings!$G$21</f>
+        <f>B11*Settings!$G$33*Settings!$G$19</f>
         <v>-0.40733649130537863</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12" s="14">
         <f>Settings!B9</f>
@@ -5091,22 +5110,22 @@
         <v>t ha-1 yr-1</v>
       </c>
       <c r="D12" s="1">
-        <f>B12*Settings!$G$35*Settings!$G$21</f>
+        <f>B12*Settings!$G$33*Settings!$G$19</f>
         <v>40.594245813869357</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13" s="14">
         <f>Settings!B19</f>
@@ -5117,22 +5136,22 @@
         <v>t yr-1</v>
       </c>
       <c r="D13" s="1">
-        <f>B13*Settings!$G$35*Settings!$G$21</f>
+        <f>B13*Settings!$G$33*Settings!$G$19</f>
         <v>46794905339.284569</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" s="14">
         <f>Settings!B21</f>
@@ -5143,22 +5162,22 @@
         <v>t yr-1</v>
       </c>
       <c r="D14" s="1">
-        <f>B14*Settings!$G$35*Settings!$G$21</f>
+        <f>B14*Settings!$G$33*Settings!$G$19</f>
         <v>3568724906.7137895</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B15" s="14">
         <f>Settings!B24</f>
@@ -5169,22 +5188,22 @@
         <v>ha emp-1</v>
       </c>
       <c r="D15" s="1">
-        <f>B15*Settings!G20</f>
+        <f>B15*Settings!G18</f>
         <v>12.35525</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B16" s="14">
         <f>Settings!B25</f>
@@ -5195,15 +5214,15 @@
         <v>$ yr-1</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B17" s="14">
         <f>Settings!B26</f>
@@ -5214,15 +5233,15 @@
         <v>opex yr-1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B18" s="14">
         <f>Settings!B22</f>
@@ -5233,22 +5252,22 @@
         <v>$ ha-1</v>
       </c>
       <c r="D18" s="1">
-        <f>B18/Settings!G$20</f>
+        <f>B18/Settings!G$18</f>
         <v>101171.56674288258</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B19" s="14">
         <f>Settings!B23</f>
@@ -5259,22 +5278,22 @@
         <v>$ ha-1</v>
       </c>
       <c r="D19" s="1">
-        <f>B19/Settings!G$20</f>
+        <f>B19/Settings!G$18</f>
         <v>404686.26697153033</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B20" s="14">
         <f>Settings!B27</f>
@@ -5285,22 +5304,22 @@
         <v>$ ha-1 yr-1</v>
       </c>
       <c r="D20" s="1">
-        <f>B20/Settings!G$20</f>
+        <f>B20/Settings!G$18</f>
         <v>13152.303676574735</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B21" s="14">
         <f>Settings!B28</f>
@@ -5311,22 +5330,22 @@
         <v>$ ha-1 yr-1</v>
       </c>
       <c r="D21" s="1">
-        <f>B21/Settings!G$20</f>
+        <f>B21/Settings!G$18</f>
         <v>28328.038688007124</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B22" s="14">
         <f>Settings!B29</f>
@@ -5337,15 +5356,15 @@
         <v>yr</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B23" s="14">
         <f>Settings!B30</f>
@@ -5356,15 +5375,15 @@
         <v>yr</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B24" s="14">
         <f>Settings!B31</f>
@@ -5375,15 +5394,15 @@
         <v>prp</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B25" s="14">
         <f>Settings!B32</f>
@@ -5394,15 +5413,15 @@
         <v>yr</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B26" s="14">
         <f>Settings!B33</f>
@@ -5413,15 +5432,15 @@
         <v>yr</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B27" s="14">
         <f>Settings!B34</f>
@@ -5432,10 +5451,10 @@
         <v>yr</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -5471,30 +5490,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>130</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" s="10">
         <v>146.7885378</v>
@@ -5503,18 +5522,18 @@
         <v>-19.257637299999999</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" s="10">
         <v>-80.457524599999999</v>
@@ -5523,21 +5542,21 @@
         <v>26.657368099999999</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3">
         <v>2009</v>
       </c>
       <c r="G3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="10">
         <v>-74.539295999999993</v>
@@ -5546,16 +5565,16 @@
         <v>40.372374000000001</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4" s="10"/>
       <c r="G4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="10">
         <v>-76.328950000000006</v>
@@ -5564,16 +5583,16 @@
         <v>37.855311</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E5" s="10"/>
       <c r="G5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B6" s="10">
         <v>-120.9</v>
@@ -5582,16 +5601,16 @@
         <v>50.8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6" s="10"/>
       <c r="G6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="10">
         <v>-119.7</v>
@@ -5600,16 +5619,16 @@
         <v>50.8</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E7" s="10"/>
       <c r="G7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="10">
         <v>-64.7</v>
@@ -5618,16 +5637,16 @@
         <v>17.45</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E8" s="10"/>
       <c r="G8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" s="10">
         <v>120.3</v>
@@ -5636,16 +5655,16 @@
         <v>23</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" s="10"/>
       <c r="G9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="10">
         <v>117.786311</v>
@@ -5654,16 +5673,16 @@
         <v>24.520453</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" s="10"/>
       <c r="G10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" s="10">
         <v>-121.132778</v>
@@ -5672,21 +5691,21 @@
         <v>37.473056</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="10">
         <v>-80.408696000000006</v>
@@ -5695,16 +5714,16 @@
         <v>27.427821999999999</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" s="10"/>
       <c r="G12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="10">
         <v>-80.427214000000006</v>
@@ -5713,16 +5732,16 @@
         <v>37.223215000000003</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14">
         <v>-79.024995599999997</v>
@@ -5731,21 +5750,21 @@
         <v>36.001745499999998</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" t="s">
         <v>152</v>
       </c>
-      <c r="F14" t="s">
-        <v>153</v>
-      </c>
       <c r="G14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15" s="10">
         <v>-80.907136899999998</v>
@@ -5754,21 +5773,21 @@
         <v>27.213987700000001</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B16">
         <v>-81.965361400000006</v>
@@ -5777,15 +5796,15 @@
         <v>27.8745254</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" s="10">
         <v>-81.880556400000003</v>
@@ -5794,21 +5813,21 @@
         <v>26.674672000000001</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F17">
         <v>2009</v>
       </c>
       <c r="G17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="10">
         <v>-80.853750700000006</v>
@@ -5817,21 +5836,21 @@
         <v>27.329125999999999</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B19">
         <v>-80.869715799999994</v>
@@ -5840,21 +5859,21 @@
         <v>27.5020904</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20">
         <v>-80.398945299999994</v>
@@ -5863,21 +5882,21 @@
         <v>27.592262000000002</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21">
         <v>-80.399409399999996</v>
@@ -5886,21 +5905,21 @@
         <v>27.602654600000001</v>
       </c>
       <c r="D21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="F21">
         <v>2010</v>
       </c>
       <c r="G21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" s="10">
         <v>-80.479466200000005</v>
@@ -5909,21 +5928,21 @@
         <v>27.609477500000001</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" s="10">
         <v>-81.445307999999997</v>
@@ -5932,21 +5951,21 @@
         <v>28.5647631</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F23">
         <v>2009</v>
       </c>
       <c r="G23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" s="10">
         <v>-82.477197000000004</v>
@@ -5955,21 +5974,21 @@
         <v>29.923072999999999</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" s="10">
         <v>-85.024425500000007</v>
@@ -5978,21 +5997,21 @@
         <v>34.827157800000002</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26">
         <v>-76.535835800000001</v>
@@ -6001,21 +6020,21 @@
         <v>39.197844400000001</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E26" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" t="s">
         <v>150</v>
       </c>
-      <c r="F26" t="s">
-        <v>151</v>
-      </c>
       <c r="G26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B27">
         <v>-76.519799699999993</v>
@@ -6024,21 +6043,21 @@
         <v>39.241779600000001</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F27">
         <v>2015</v>
       </c>
       <c r="G27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B28">
         <v>-76.262986100000006</v>
@@ -6047,21 +6066,21 @@
         <v>39.7560024</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F28">
         <v>2009</v>
       </c>
       <c r="G28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" s="10">
         <v>-73.828925999999996</v>
@@ -6070,21 +6089,21 @@
         <v>40.584173399999997</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B30" s="10">
         <v>3.5740601999999999</v>
@@ -6093,16 +6112,16 @@
         <v>51.082552</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" s="10"/>
       <c r="G30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31" s="10">
         <v>16.430962999999998</v>
@@ -6111,16 +6130,16 @@
         <v>48.197578999999998</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>146.80000000000001</v>
@@ -6129,12 +6148,12 @@
         <v>-19.3</v>
       </c>
       <c r="G32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="10">
         <v>-76.900000000000006</v>
@@ -6143,16 +6162,16 @@
         <v>39</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E33" s="10"/>
       <c r="G33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="10">
         <v>-76.713593000000003</v>
@@ -6161,16 +6180,16 @@
         <v>38.784427000000001</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E34" s="10"/>
       <c r="G34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35">
         <v>-76.457588999999999</v>
@@ -6179,15 +6198,15 @@
         <v>39.131529</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36">
         <v>-76.268676999999997</v>
@@ -6196,15 +6215,15 @@
         <v>39.449888999999999</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="10">
         <v>-76.188846600000005</v>
@@ -6213,16 +6232,16 @@
         <v>38.609043200000002</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E37" s="10"/>
       <c r="G37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="10">
         <v>-76.382262999999995</v>
@@ -6231,21 +6250,21 @@
         <v>37.247632000000003</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="10">
         <v>-94.1666666666667</v>
@@ -6254,21 +6273,21 @@
         <v>36.200000000000003</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F39">
         <v>2009</v>
       </c>
       <c r="G39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="10">
         <v>-94.089297000000002</v>
@@ -6277,21 +6296,21 @@
         <v>36.080810999999997</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="10">
         <v>-82.323492000000002</v>
@@ -6300,16 +6319,16 @@
         <v>29.645575999999998</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E41" s="10"/>
       <c r="G41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B42" s="10">
         <v>-98.806156999999999</v>
@@ -6318,21 +6337,21 @@
         <v>29.491195399999999</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B43" s="10">
         <v>16.163287777777775</v>
@@ -6341,16 +6360,16 @@
         <v>51.627626666666664</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E43" s="10"/>
       <c r="G43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B44">
         <v>-103.3499748</v>
@@ -6359,21 +6378,21 @@
         <v>34.178595899999998</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B45" s="10">
         <v>-75.900000000000006</v>
@@ -6382,11 +6401,11 @@
         <v>39</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E45" s="10"/>
       <c r="G45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6414,10 +6433,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6442,28 +6461,28 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="23" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2" s="17">
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D2" s="16"/>
       <c r="F2" s="16" t="s">
@@ -6486,7 +6505,7 @@
         <v>54.787500000000001</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="16"/>
       <c r="F3" s="16" t="s">
@@ -6497,18 +6516,18 @@
         <v>10000</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="17">
         <v>25</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="16"/>
       <c r="F4" s="16" t="s">
@@ -6531,11 +6550,11 @@
         <v>91.3125</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G5" s="13">
         <v>1000</v>
@@ -6546,13 +6565,13 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B6" s="13">
         <v>40</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" s="12"/>
       <c r="F6" s="12" t="s">
@@ -6567,17 +6586,17 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B7" s="13">
         <v>0</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G7" s="13">
         <v>1000</v>
@@ -6588,21 +6607,21 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B8" s="13">
         <f>(B5-B3)/(B7-B6)</f>
         <v>-0.91312499999999996</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="12"/>
       <c r="F8" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="1">
-        <f>(G9+2*G11)/G9</f>
+        <f>(G9+2*G12)/G9</f>
         <v>3.6641245524935475</v>
       </c>
       <c r="H8" t="s">
@@ -6611,17 +6630,17 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B9" s="13">
         <v>91</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" s="13">
         <v>12.010999999999999</v>
@@ -6632,7 +6651,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B10" s="13">
         <v>410</v>
@@ -6642,10 +6661,10 @@
       </c>
       <c r="D10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>70</v>
+        <v>313</v>
       </c>
       <c r="G10" s="13">
-        <v>14.007</v>
+        <v>1.008</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>5</v>
@@ -6653,10 +6672,10 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B11" s="17">
-        <f>B10*G33</f>
+        <f>B10*G31</f>
         <v>873300000000</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -6664,10 +6683,10 @@
       </c>
       <c r="D11" s="17"/>
       <c r="F11" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G11" s="13">
-        <v>15.9994</v>
+        <v>14.007</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>5</v>
@@ -6675,22 +6694,22 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B12" s="13">
         <v>2</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G12" s="13">
-        <v>30.97</v>
+        <v>15.9994</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>5</v>
@@ -6699,71 +6718,64 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B13" s="17">
-        <f>B12*G33</f>
+        <f>B12*G31</f>
         <v>4260000000</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="16"/>
       <c r="F13" s="12" t="s">
-        <v>112</v>
+        <v>70</v>
       </c>
       <c r="G13" s="13">
-        <v>0.5</v>
+        <v>30.97</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" t="s">
-        <v>311</v>
+        <v>5</v>
       </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11">
       <c r="F14" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G14" s="13">
-        <v>4.8000000000000001E-2</v>
+        <f>D38</f>
+        <v>0.35830664911296195</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="I14" t="s">
-        <v>311</v>
+        <v>108</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G15" s="13">
-        <v>3.0000000000000001E-3</v>
+        <f>D41</f>
+        <v>6.3071759492481047E-2</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="I15" t="s">
-        <v>311</v>
+        <v>109</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B16" s="19">
         <v>5</v>
@@ -6772,20 +6784,17 @@
         <v>2</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G16" s="13">
-        <f>D38</f>
-        <v>0.83308860865513967</v>
+        <f>D42</f>
+        <v>8.7158759525689748E-3</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="I16" t="s">
-        <v>312</v>
+        <v>110</v>
       </c>
       <c r="K16" s="1"/>
     </row>
@@ -6797,121 +6806,114 @@
         <v>75845109000000</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" s="13">
-        <f>D39</f>
-        <v>0.1466463558270647</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" t="s">
-        <v>312</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0.26417200000000002</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="1"/>
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" s="13">
         <v>104.9</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="13">
-        <f>D40</f>
-        <v>2.026503551779554E-2</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="I18" t="s">
-        <v>312</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="14">
+        <v>2.47105</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" s="17">
         <f>B18*$G$6/$G$4</f>
         <v>104900000000</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="16"/>
       <c r="F19" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G19" s="14">
-        <v>0.26417200000000002</v>
+        <f>1/G18</f>
+        <v>0.40468626697153032</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I19" s="1"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B20" s="13">
         <v>8</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="G20" s="14">
-        <v>2.47105</v>
+        <f>1/2.54</f>
+        <v>0.39370078740157477</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20" s="1"/>
+        <v>89</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B21" s="17">
         <f>B20*$G$6/$G$4</f>
         <v>8000000000</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="16"/>
       <c r="F21" s="5" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="G21" s="14">
-        <f>1/G20</f>
-        <v>0.40468626697153032</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>2</v>
+        <v>3.28084</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -6922,20 +6924,19 @@
         <v>250000</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>89</v>
+        <v>206</v>
       </c>
       <c r="G22" s="14">
-        <f>1/2.54</f>
-        <v>0.39370078740157477</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>90</v>
+        <v>1.3079499999999999</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>207</v>
       </c>
       <c r="K22" s="1"/>
     </row>
@@ -6947,19 +6948,20 @@
         <v>1000000</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>185</v>
+        <v>90</v>
       </c>
       <c r="G23" s="14">
-        <v>3.28084</v>
+        <f>1000000*G24/2000</f>
+        <v>1.1023099999999999</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="K23" s="1"/>
     </row>
@@ -6971,20 +6973,21 @@
         <v>5</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="5" t="s">
-        <v>207</v>
+        <v>5</v>
       </c>
       <c r="G24" s="14">
-        <v>1.3079499999999999</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>208</v>
+        <f>0.00220462</f>
+        <v>2.20462E-3</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="K24" s="1"/>
     </row>
@@ -6996,20 +6999,19 @@
         <v>100000</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="G25" s="14">
-        <f>1000000*G26/2000</f>
-        <v>1.1023099999999999</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>4</v>
+        <v>9.2902999999999998E-6</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -7020,20 +7022,19 @@
         <v>0.05</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="G26" s="14">
-        <f>0.00220462</f>
-        <v>2.20462E-3</v>
+        <v>5280</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -7045,18 +7046,19 @@
         <v>32500</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" s="12"/>
       <c r="F27" s="5" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="G27" s="14">
-        <v>9.2902999999999998E-6</v>
+        <v>0.453592</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="12" t="s">
@@ -7067,22 +7069,22 @@
         <v>70000</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" s="12"/>
       <c r="F28" s="5" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="G28" s="14">
-        <v>5280</v>
+        <v>6.4515999999999998E-4</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B29" s="13">
         <v>40</v>
@@ -7091,22 +7093,21 @@
         <v>0</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="14">
-        <v>0.453592</v>
+        <v>14</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1.60934</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I29" s="1"/>
+        <v>265</v>
+      </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" s="13">
         <v>20</v>
@@ -7115,16 +7116,16 @@
         <v>0</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>103</v>
+        <v>265</v>
       </c>
       <c r="G30" s="14">
-        <v>6.4515999999999998E-4</v>
+        <v>1000</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>102</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -7135,24 +7136,24 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="5">
-        <v>1.60934</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>266</v>
+        <v>260</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="G31" s="17">
+        <v>2130000000</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B32" s="13">
         <v>50</v>
@@ -7161,21 +7162,22 @@
         <v>0</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>266</v>
+        <v>4</v>
       </c>
       <c r="G32" s="14">
-        <v>1000</v>
+        <f>1000/G27</f>
+        <v>2204.6244201837776</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>185</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B33" s="13">
         <v>100</v>
@@ -7184,21 +7186,22 @@
         <v>0</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="F33" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="14">
+        <f>G32/2000</f>
+        <v>1.1023122100918887</v>
+      </c>
+      <c r="H33" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="G33" s="17">
-        <v>2130000000</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B34" s="13">
         <v>200</v>
@@ -7207,17 +7210,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G34" s="14">
-        <f>1000/G29</f>
-        <v>2204.6244201837776</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -7225,20 +7218,10 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="F35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G35" s="14">
-        <f>G34/2000</f>
-        <v>1.1023122100918887</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="25" t="s">
-        <v>64</v>
+        <v>312</v>
       </c>
       <c r="B36" s="25"/>
       <c r="C36" s="25"/>
@@ -7247,16 +7230,16 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="C37" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -7271,50 +7254,82 @@
         <v>1273.1659999999999</v>
       </c>
       <c r="D38" s="14">
-        <f>C38/C$41</f>
-        <v>0.83308860865513967</v>
+        <f>C38/C$43</f>
+        <v>0.35830664911296195</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="5" t="s">
-        <v>8</v>
+        <v>310</v>
       </c>
       <c r="B39" s="14">
-        <v>16</v>
+        <v>263</v>
       </c>
       <c r="C39" s="14">
         <f>G10*B39</f>
+        <v>265.10399999999998</v>
+      </c>
+      <c r="D39" s="14">
+        <f>C39/C$43</f>
+        <v>7.4608123297702472E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B40" s="14">
+        <v>110</v>
+      </c>
+      <c r="C40" s="14">
+        <f>G12*B40</f>
+        <v>1759.934</v>
+      </c>
+      <c r="D40" s="14">
+        <f>C40/C$43</f>
+        <v>0.49529759214428565</v>
+      </c>
+      <c r="M40" s="9"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="14">
+        <v>16</v>
+      </c>
+      <c r="C41" s="14">
+        <f>G11*B41</f>
         <v>224.11199999999999</v>
       </c>
-      <c r="D39" s="14">
-        <f>C39/C$41</f>
-        <v>0.1466463558270647</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" t="s">
+      <c r="D41" s="14">
+        <f>C41/C$43</f>
+        <v>6.3071759492481047E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B42" s="1">
         <v>1</v>
       </c>
-      <c r="C40" s="1">
-        <f>G12*B40</f>
+      <c r="C42" s="1">
+        <f>G13*B42</f>
         <v>30.97</v>
       </c>
-      <c r="D40" s="1">
-        <f>C40/C$41</f>
-        <v>2.026503551779554E-2</v>
-      </c>
-      <c r="M40" s="9"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1">
-        <f>SUM(C38:C40)</f>
-        <v>1528.248</v>
-      </c>
-      <c r="D41" s="1"/>
+      <c r="D42" s="1">
+        <f>C42/C$43</f>
+        <v>8.7158759525689748E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1">
+        <f>SUM(C38:C42)</f>
+        <v>3553.2859999999996</v>
+      </c>
+      <c r="D43" s="1"/>
     </row>
     <row r="57" spans="5:5">
       <c r="E57" s="1"/>
@@ -7322,17 +7337,17 @@
     <row r="60" spans="5:5">
       <c r="E60" s="1"/>
     </row>
-    <row r="83" spans="8:9">
-      <c r="H83" s="6"/>
-    </row>
-    <row r="84" spans="8:9">
-      <c r="H84" s="7"/>
-    </row>
-    <row r="92" spans="8:9">
-      <c r="I92" s="4"/>
-    </row>
-    <row r="93" spans="8:9">
-      <c r="I93" s="8"/>
+    <row r="80" spans="8:8">
+      <c r="H80" s="6"/>
+    </row>
+    <row r="81" spans="8:9">
+      <c r="H81" s="7"/>
+    </row>
+    <row r="89" spans="8:9">
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="8:9">
+      <c r="I90" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7384,10 +7399,10 @@
         <v>21</v>
       </c>
       <c r="R1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
@@ -7430,10 +7445,10 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="S2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -7482,13 +7497,13 @@
         <v>26</v>
       </c>
       <c r="R3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S3" s="1">
         <v>53.4</v>
       </c>
       <c r="T3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -7537,14 +7552,14 @@
         <v>27</v>
       </c>
       <c r="R4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S4" s="1">
         <f>'R Variables'!$B$11*Wetlands!S3+'R Variables'!$B$12</f>
         <v>42.239125000000001</v>
       </c>
       <c r="T4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -7590,7 +7605,7 @@
         <v>2.8</v>
       </c>
       <c r="T5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -7636,7 +7651,7 @@
         <v>0.35</v>
       </c>
       <c r="T6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -7682,7 +7697,7 @@
         <v>0.97999999999999987</v>
       </c>
       <c r="T7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -7719,13 +7734,13 @@
         <v>3785.41</v>
       </c>
       <c r="R8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S8" s="1">
         <v>0.4</v>
       </c>
       <c r="T8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -7771,7 +7786,7 @@
         <v>0.26</v>
       </c>
       <c r="T9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -7808,7 +7823,7 @@
         <v>0.10400000000000001</v>
       </c>
       <c r="T10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -7838,26 +7853,26 @@
       </c>
       <c r="L11" s="2"/>
       <c r="R11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S11" s="1">
-        <f>S7/Settings!G14</f>
-        <v>20.416666666666664</v>
+        <f>S7/Settings!G15</f>
+        <v>15.537857321339327</v>
       </c>
       <c r="T11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="R12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S12" s="1">
-        <f>S10/Settings!$G$15</f>
-        <v>34.666666666666671</v>
+        <f>S10/Settings!$G$16</f>
+        <v>11.93224875686148</v>
       </c>
       <c r="T12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -7871,81 +7886,81 @@
       </c>
       <c r="L13" s="2"/>
       <c r="R13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="S13" s="1">
         <f>$S$4/S11</f>
-        <v>2.0688551020408168</v>
+        <v>2.7184652379314733</v>
       </c>
       <c r="T13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="R14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S14" s="1">
         <f>$S$4/S12</f>
-        <v>1.218436298076923</v>
+        <v>3.5399132100486055</v>
       </c>
       <c r="T14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="R16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="18:20">
       <c r="R17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="18:20">
       <c r="R18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S18" s="1">
         <v>7.3</v>
       </c>
       <c r="T18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="18:20">
       <c r="R19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S19" s="1">
         <f>'R Variables'!$B$11*Wetlands!S18+'R Variables'!$B$12</f>
         <v>84.334187499999999</v>
       </c>
       <c r="T19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="18:20">
       <c r="R20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S20" s="1">
         <v>25</v>
       </c>
       <c r="T20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="18:20">
       <c r="R21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S21" s="1">
         <f>S20/Settings!G3</f>
@@ -7957,48 +7972,48 @@
     </row>
     <row r="22" spans="18:20">
       <c r="R22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S22" s="1">
         <v>13</v>
       </c>
       <c r="T22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="18:20">
       <c r="R23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S23" s="1">
         <f>S22*Settings!$G$7</f>
         <v>13000</v>
       </c>
       <c r="T23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="18:20">
       <c r="R24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S24" s="1">
         <v>1.36</v>
       </c>
       <c r="T24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="18:20">
       <c r="R25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S25" s="1">
         <f>S24*$S$23</f>
         <v>17680</v>
       </c>
       <c r="T25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="18:20">
@@ -8009,7 +8024,7 @@
         <v>0.19</v>
       </c>
       <c r="T26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="18:20">
@@ -8021,7 +8036,7 @@
         <v>3359.2</v>
       </c>
       <c r="T27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="18:20">
@@ -8033,7 +8048,7 @@
         <v>1226947.8</v>
       </c>
       <c r="T28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="18:20">
@@ -8045,7 +8060,7 @@
         <v>#REF!</v>
       </c>
       <c r="T29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="18:20">
@@ -8057,63 +8072,63 @@
         <v>#REF!</v>
       </c>
       <c r="T30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="18:20">
       <c r="R31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S31" s="1" t="e">
-        <f>S30/Settings!$G$15</f>
+        <f>S30/Settings!$G$16</f>
         <v>#REF!</v>
       </c>
       <c r="T31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="18:20">
       <c r="R33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="18:20">
       <c r="R34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="18:20">
       <c r="R35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S35" s="1">
         <v>24.8</v>
       </c>
       <c r="T35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="18:20">
       <c r="R36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S36" s="1">
         <f>'R Variables'!$B$11*Wetlands!S35+'R Variables'!$B$12</f>
         <v>68.354500000000002</v>
       </c>
       <c r="T36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="18:20">
       <c r="R37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S37" s="1">
         <v>1.07</v>
@@ -8124,48 +8139,48 @@
     </row>
     <row r="38" spans="18:20">
       <c r="R38" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S38" s="1">
         <v>4000</v>
       </c>
       <c r="T38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="18:20">
       <c r="R39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S39" s="1">
         <f>S38*Settings!$G$7</f>
         <v>4000000</v>
       </c>
       <c r="T39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="18:20">
       <c r="R40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S40" s="1">
         <v>1.9</v>
       </c>
       <c r="T40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="18:20">
       <c r="R41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S41" s="1">
         <f>S40*$S$23</f>
         <v>24700</v>
       </c>
       <c r="T41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="18:20">
@@ -8176,7 +8191,7 @@
         <v>0.44</v>
       </c>
       <c r="T42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="18:20">
@@ -8188,7 +8203,7 @@
         <v>10868</v>
       </c>
       <c r="T43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="18:20">
@@ -8200,7 +8215,7 @@
         <v>3969537</v>
       </c>
       <c r="T44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="18:20">
@@ -8212,7 +8227,7 @@
         <v>#REF!</v>
       </c>
       <c r="T45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="18:20">
@@ -8224,19 +8239,19 @@
         <v>#REF!</v>
       </c>
       <c r="T46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="18:20">
       <c r="R47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S47" s="1" t="e">
-        <f>S46/Settings!$G$15</f>
+        <f>S46/Settings!$G$16</f>
         <v>#REF!</v>
       </c>
       <c r="T47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="18:20">
@@ -8244,7 +8259,7 @@
         <v>23</v>
       </c>
       <c r="T51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -8276,7 +8291,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>62</v>
@@ -8285,12 +8300,12 @@
         <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B2" s="1">
         <f>[1]A!$R$66</f>
@@ -8300,24 +8315,24 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B3" s="1">
-        <f>'Highway Costs'!B2*Settings!G32*Settings!G31</f>
+        <f>'Highway Costs'!B2*Settings!G30*Settings!G29</f>
         <v>14107553603.434601</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -8326,24 +8341,24 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B5" s="1">
-        <f>B4/Settings!G23</f>
+        <f>B4/Settings!G21</f>
         <v>3.6575998829568039</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B6" s="1">
         <f>B5*B3</f>
@@ -8355,7 +8370,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B7" s="1">
         <f>B6/Settings!G3</f>
@@ -8367,56 +8382,56 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B8" s="1">
         <f>1000*[2]HF2!$E$67</f>
         <v>105423740057.83682</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B9" s="1">
         <f>1000*[2]HF2!$I$67</f>
         <v>51442240042.163231</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B10" s="1">
         <f>B9+B8</f>
         <v>156865980100.00006</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B11" s="1">
         <f>B10/B7</f>
         <v>30400.509579137084</v>
       </c>
       <c r="C11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:4">

</xml_diff>

<commit_message>
Fix baseline CO2 (which should be baseline C) and mean_prod
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="314">
   <si>
     <t>yr</t>
   </si>
@@ -1081,8 +1081,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1627">
+  <cellStyleXfs count="1629">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2752,7 +2754,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1627">
+  <cellStyles count="1629">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3566,6 +3568,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1622" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1628" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4379,6 +4382,7 @@
     <cellStyle name="Hyperlink" xfId="1621" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1627" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4820,7 +4824,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4940,15 +4944,19 @@
         <v>237</v>
       </c>
       <c r="B5" s="14">
-        <f>Settings!B10</f>
-        <v>410</v>
-      </c>
-      <c r="C5" s="14" t="str">
-        <f>Settings!C10</f>
-        <v>ppm</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+        <f>Settings!B11</f>
+        <v>873300000000</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <f>B5*Settings!G$33</f>
+        <v>962649253073.24646</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="F5" s="5" t="s">
         <v>121</v>
       </c>
@@ -4961,15 +4969,19 @@
         <v>238</v>
       </c>
       <c r="B6" s="14">
-        <f>Settings!B12</f>
-        <v>2</v>
-      </c>
-      <c r="C6" s="14" t="str">
-        <f>Settings!C12</f>
-        <v>ppm yr-1</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+        <f>Settings!B13</f>
+        <v>4260000000</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6*Settings!G$33</f>
+        <v>4695850014.9914455</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="F6" s="5" t="s">
         <v>120</v>
       </c>
@@ -6435,8 +6447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Getting generated paragraph 1 into shape.
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="316">
   <si>
     <t>yr</t>
   </si>
@@ -969,6 +969,12 @@
   </si>
   <si>
     <t>mol H</t>
+  </si>
+  <si>
+    <t>t ha-1</t>
+  </si>
+  <si>
+    <t>T ac</t>
   </si>
 </sst>
 </file>
@@ -1081,7 +1087,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1629">
+  <cellStyleXfs count="1633">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2711,8 +2717,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2753,8 +2763,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1629">
+  <cellStyles count="1633">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3569,6 +3580,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1626" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1632" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4383,6 +4396,8 @@
     <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1625" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1631" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4824,7 +4839,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6447,8 +6462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7224,12 +7239,24 @@
       <c r="D34" s="12" t="s">
         <v>260</v>
       </c>
+      <c r="F34" s="12" t="s">
+        <v>314</v>
+      </c>
+      <c r="G34" s="1">
+        <f>G33*G18</f>
+        <v>2.7238685867475616</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="I34" s="26"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
+      <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="25" t="s">

</xml_diff>

<commit_message>
To coauthors for review.
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764" activeTab="2"/>
+    <workbookView xWindow="7240" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764"/>
   </bookViews>
   <sheets>
     <sheet name="R Variables" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="317">
   <si>
     <t>yr</t>
   </si>
@@ -975,6 +975,9 @@
   </si>
   <si>
     <t>T ac</t>
+  </si>
+  <si>
+    <t>world_dp</t>
   </si>
 </sst>
 </file>
@@ -2751,6 +2754,7 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2763,7 +2767,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1633">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4836,10 +4839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5482,6 +5485,18 @@
       </c>
       <c r="G27" s="5" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B28" s="1">
+        <f>Settings!B17</f>
+        <v>75845109000000</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -6462,7 +6477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
@@ -6487,19 +6502,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="16" t="s">
@@ -6780,11 +6795,11 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="15" t="s">
         <v>212</v>
       </c>
@@ -7249,7 +7264,7 @@
       <c r="H34" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="I34" s="26"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="5"/>
@@ -7259,12 +7274,12 @@
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:13">

</xml_diff>

<commit_message>
Final commit for Heliyon
</commit_message>
<xml_diff>
--- a/Data/Spreadsheets/EACCRPBT.xlsx
+++ b/Data/Spreadsheets/EACCRPBT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764"/>
+    <workbookView xWindow="7240" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="764" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="R Variables" sheetId="12" r:id="rId1"/>
@@ -389,12 +389,6 @@
     <t>P:biomass ratio</t>
   </si>
   <si>
-    <t>Growth rate, atmospheric CO2</t>
-  </si>
-  <si>
-    <t>Baseline CO2 mass, atmosphere</t>
-  </si>
-  <si>
     <t>Kangas and Mulbry, 2013</t>
   </si>
   <si>
@@ -740,12 +734,6 @@
     <t>P_prp</t>
   </si>
   <si>
-    <t>CO2_bl</t>
-  </si>
-  <si>
-    <t>CO2_gr</t>
-  </si>
-  <si>
     <t>mod_lat_hi</t>
   </si>
   <si>
@@ -978,6 +966,18 @@
   </si>
   <si>
     <t>world_dp</t>
+  </si>
+  <si>
+    <t>Baseline C mass, atmosphere</t>
+  </si>
+  <si>
+    <t>Growth rate, atmospheric C</t>
+  </si>
+  <si>
+    <t>C_bl</t>
+  </si>
+  <si>
+    <t>C_gr</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1037,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1056,30 +1056,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2725,7 +2701,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2742,18 +2718,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4841,8 +4809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4860,17 +4828,17 @@
       <c r="A1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>94</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>107</v>
@@ -4881,13 +4849,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B2" s="14">
+        <v>232</v>
+      </c>
+      <c r="B2" s="12">
         <f>Settings!G14</f>
         <v>0.35830664911296195</v>
       </c>
-      <c r="C2" s="14" t="str">
+      <c r="C2" s="12" t="str">
         <f>Settings!H14&amp;" "&amp;Settings!F14&amp;"-1"</f>
         <v>gC gBiomass-1</v>
       </c>
@@ -4896,7 +4864,7 @@
         <v>0.35830664911296195</v>
       </c>
       <c r="E2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>117</v>
@@ -4907,13 +4875,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B3" s="14">
+        <v>233</v>
+      </c>
+      <c r="B3" s="12">
         <f>Settings!G15</f>
         <v>6.3071759492481047E-2</v>
       </c>
-      <c r="C3" s="14" t="str">
+      <c r="C3" s="12" t="str">
         <f>Settings!H15&amp;" "&amp;Settings!F15&amp;"-1"</f>
         <v>gN gBiomass-1</v>
       </c>
@@ -4922,7 +4890,7 @@
         <v>6.3071759492481047E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>118</v>
@@ -4933,13 +4901,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B4" s="14">
+        <v>234</v>
+      </c>
+      <c r="B4" s="12">
         <f>Settings!G16</f>
         <v>8.7158759525689748E-3</v>
       </c>
-      <c r="C4" s="14" t="str">
+      <c r="C4" s="12" t="str">
         <f>Settings!H16&amp;" "&amp;Settings!F16&amp;"-1"</f>
         <v>gP gBiomass-1</v>
       </c>
@@ -4948,7 +4916,7 @@
         <v>8.7158759525689748E-3</v>
       </c>
       <c r="E4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>119</v>
@@ -4959,13 +4927,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B5" s="14">
+        <v>315</v>
+      </c>
+      <c r="B5" s="12">
         <f>Settings!B11</f>
         <v>873300000000</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="1">
@@ -4973,10 +4941,10 @@
         <v>962649253073.24646</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>121</v>
+        <v>313</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>114</v>
@@ -4984,13 +4952,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B6" s="14">
+        <v>316</v>
+      </c>
+      <c r="B6" s="12">
         <f>Settings!B13</f>
         <v>4260000000</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>99</v>
       </c>
       <c r="D6" s="1">
@@ -4998,10 +4966,10 @@
         <v>4695850014.9914455</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>120</v>
+        <v>314</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>114</v>
@@ -5009,13 +4977,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="14">
+        <v>235</v>
+      </c>
+      <c r="B7" s="12">
         <f>Settings!B6</f>
         <v>40</v>
       </c>
-      <c r="C7" s="14" t="str">
+      <c r="C7" s="12" t="str">
         <f>Settings!C6</f>
         <v>deg</v>
       </c>
@@ -5030,20 +4998,20 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B8" s="14">
+        <v>236</v>
+      </c>
+      <c r="B8" s="12">
         <f>Settings!B7</f>
         <v>0</v>
       </c>
-      <c r="C8" s="14" t="str">
+      <c r="C8" s="12" t="str">
         <f>Settings!C7</f>
         <v>deg</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>114</v>
@@ -5051,13 +5019,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B9" s="14">
+        <v>250</v>
+      </c>
+      <c r="B9" s="12">
         <f>Settings!B3</f>
         <v>54.787500000000001</v>
       </c>
-      <c r="C9" s="14" t="str">
+      <c r="C9" s="12" t="str">
         <f>Settings!C3</f>
         <v>t ha-1 yr-1</v>
       </c>
@@ -5066,10 +5034,10 @@
         <v>24.440189478322718</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>114</v>
@@ -5077,13 +5045,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B10" s="14">
+        <v>251</v>
+      </c>
+      <c r="B10" s="12">
         <f>Settings!B5</f>
         <v>91.3125</v>
       </c>
-      <c r="C10" s="14" t="str">
+      <c r="C10" s="12" t="str">
         <f>Settings!C5</f>
         <v>t ha-1 yr-1</v>
       </c>
@@ -5092,10 +5060,10 @@
         <v>40.733649130537863</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>114</v>
@@ -5103,13 +5071,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B11" s="14">
+        <v>237</v>
+      </c>
+      <c r="B11" s="12">
         <f>Settings!B8</f>
         <v>-0.91312499999999996</v>
       </c>
-      <c r="C11" s="14" t="str">
+      <c r="C11" s="12" t="str">
         <f>Settings!C8</f>
         <v>t ha-1 yr-1 deg-1</v>
       </c>
@@ -5118,7 +5086,7 @@
         <v>-0.40733649130537863</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>116</v>
@@ -5129,13 +5097,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B12" s="14">
+        <v>238</v>
+      </c>
+      <c r="B12" s="12">
         <f>Settings!B9</f>
         <v>91</v>
       </c>
-      <c r="C12" s="14" t="str">
+      <c r="C12" s="12" t="str">
         <f>Settings!C5</f>
         <v>t ha-1 yr-1</v>
       </c>
@@ -5144,10 +5112,10 @@
         <v>40.594245813869357</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>114</v>
@@ -5155,13 +5123,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B13" s="14">
+        <v>239</v>
+      </c>
+      <c r="B13" s="12">
         <f>Settings!B19</f>
         <v>104900000000</v>
       </c>
-      <c r="C13" s="14" t="str">
+      <c r="C13" s="12" t="str">
         <f>Settings!C19</f>
         <v>t yr-1</v>
       </c>
@@ -5170,10 +5138,10 @@
         <v>46794905339.284569</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>114</v>
@@ -5181,13 +5149,13 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="B14" s="14">
+        <v>240</v>
+      </c>
+      <c r="B14" s="12">
         <f>Settings!B21</f>
         <v>8000000000</v>
       </c>
-      <c r="C14" s="14" t="str">
+      <c r="C14" s="12" t="str">
         <f>Settings!C21</f>
         <v>t yr-1</v>
       </c>
@@ -5196,10 +5164,10 @@
         <v>3568724906.7137895</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>114</v>
@@ -5207,13 +5175,13 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B15" s="14">
+        <v>241</v>
+      </c>
+      <c r="B15" s="12">
         <f>Settings!B24</f>
         <v>5</v>
       </c>
-      <c r="C15" s="14" t="str">
+      <c r="C15" s="12" t="str">
         <f>Settings!C24</f>
         <v>ha emp-1</v>
       </c>
@@ -5222,10 +5190,10 @@
         <v>12.35525</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>113</v>
@@ -5233,18 +5201,18 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B16" s="14">
+        <v>242</v>
+      </c>
+      <c r="B16" s="12">
         <f>Settings!B25</f>
         <v>100000</v>
       </c>
-      <c r="C16" s="14" t="str">
+      <c r="C16" s="12" t="str">
         <f>Settings!C25</f>
         <v>$ yr-1</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>113</v>
@@ -5252,18 +5220,18 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B17" s="14">
+        <v>243</v>
+      </c>
+      <c r="B17" s="12">
         <f>Settings!B26</f>
         <v>0.05</v>
       </c>
-      <c r="C17" s="14" t="str">
+      <c r="C17" s="12" t="str">
         <f>Settings!C26</f>
         <v>opex yr-1</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>113</v>
@@ -5271,13 +5239,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B18" s="14">
+        <v>244</v>
+      </c>
+      <c r="B18" s="12">
         <f>Settings!B22</f>
         <v>250000</v>
       </c>
-      <c r="C18" s="14" t="str">
+      <c r="C18" s="12" t="str">
         <f>Settings!C22</f>
         <v>$ ha-1</v>
       </c>
@@ -5286,10 +5254,10 @@
         <v>101171.56674288258</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>113</v>
@@ -5297,13 +5265,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B19" s="14">
+        <v>245</v>
+      </c>
+      <c r="B19" s="12">
         <f>Settings!B23</f>
         <v>1000000</v>
       </c>
-      <c r="C19" s="14" t="str">
+      <c r="C19" s="12" t="str">
         <f>Settings!C23</f>
         <v>$ ha-1</v>
       </c>
@@ -5312,10 +5280,10 @@
         <v>404686.26697153033</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>113</v>
@@ -5323,13 +5291,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="B20" s="14">
+        <v>246</v>
+      </c>
+      <c r="B20" s="12">
         <f>Settings!B27</f>
         <v>32500</v>
       </c>
-      <c r="C20" s="14" t="str">
+      <c r="C20" s="12" t="str">
         <f>Settings!C27</f>
         <v>$ ha-1 yr-1</v>
       </c>
@@ -5338,10 +5306,10 @@
         <v>13152.303676574735</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>113</v>
@@ -5349,13 +5317,13 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="B21" s="14">
+        <v>247</v>
+      </c>
+      <c r="B21" s="12">
         <f>Settings!B28</f>
         <v>70000</v>
       </c>
-      <c r="C21" s="14" t="str">
+      <c r="C21" s="12" t="str">
         <f>Settings!C28</f>
         <v>$ ha-1 yr-1</v>
       </c>
@@ -5364,10 +5332,10 @@
         <v>28328.038688007124</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>113</v>
@@ -5375,18 +5343,18 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B22" s="14">
+        <v>248</v>
+      </c>
+      <c r="B22" s="12">
         <f>Settings!B29</f>
         <v>40</v>
       </c>
-      <c r="C22" s="14" t="str">
+      <c r="C22" s="12" t="str">
         <f>Settings!C29</f>
         <v>yr</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>113</v>
@@ -5394,18 +5362,18 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B23" s="14">
+        <v>249</v>
+      </c>
+      <c r="B23" s="12">
         <f>Settings!B30</f>
         <v>20</v>
       </c>
-      <c r="C23" s="14" t="str">
+      <c r="C23" s="12" t="str">
         <f>Settings!C30</f>
         <v>yr</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>113</v>
@@ -5413,18 +5381,18 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B24" s="14">
+        <v>252</v>
+      </c>
+      <c r="B24" s="12">
         <f>Settings!B31</f>
         <v>0.1</v>
       </c>
-      <c r="C24" s="14" t="str">
+      <c r="C24" s="12" t="str">
         <f>Settings!C31</f>
         <v>prp</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>113</v>
@@ -5432,18 +5400,18 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B25" s="14">
+        <v>253</v>
+      </c>
+      <c r="B25" s="12">
         <f>Settings!B32</f>
         <v>50</v>
       </c>
-      <c r="C25" s="14" t="str">
+      <c r="C25" s="12" t="str">
         <f>Settings!C32</f>
         <v>yr</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>113</v>
@@ -5451,18 +5419,18 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B26" s="14">
+        <v>254</v>
+      </c>
+      <c r="B26" s="12">
         <f>Settings!B33</f>
         <v>100</v>
       </c>
-      <c r="C26" s="14" t="str">
+      <c r="C26" s="12" t="str">
         <f>Settings!C33</f>
         <v>yr</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>113</v>
@@ -5470,18 +5438,18 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B27" s="14">
+        <v>255</v>
+      </c>
+      <c r="B27" s="12">
         <f>Settings!B34</f>
         <v>200</v>
       </c>
-      <c r="C27" s="14" t="str">
+      <c r="C27" s="12" t="str">
         <f>Settings!C34</f>
         <v>yr</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>113</v>
@@ -5489,7 +5457,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B28" s="1">
         <f>Settings!B17</f>
@@ -5532,30 +5500,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>129</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" s="10">
         <v>146.7885378</v>
@@ -5564,18 +5532,18 @@
         <v>-19.257637299999999</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" s="10">
         <v>-80.457524599999999</v>
@@ -5584,21 +5552,21 @@
         <v>26.657368099999999</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F3">
         <v>2009</v>
       </c>
       <c r="G3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B4" s="10">
         <v>-74.539295999999993</v>
@@ -5607,11 +5575,11 @@
         <v>40.372374000000001</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E4" s="10"/>
       <c r="G4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5625,16 +5593,16 @@
         <v>37.855311</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" s="10"/>
       <c r="G5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B6" s="10">
         <v>-120.9</v>
@@ -5643,16 +5611,16 @@
         <v>50.8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E6" s="10"/>
       <c r="G6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" s="10">
         <v>-119.7</v>
@@ -5661,11 +5629,11 @@
         <v>50.8</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E7" s="10"/>
       <c r="G7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -5679,16 +5647,16 @@
         <v>17.45</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" s="10"/>
       <c r="G8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B9" s="10">
         <v>120.3</v>
@@ -5697,11 +5665,11 @@
         <v>23</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" s="10"/>
       <c r="G9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -5715,16 +5683,16 @@
         <v>24.520453</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E10" s="10"/>
       <c r="G10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B11" s="10">
         <v>-121.132778</v>
@@ -5733,16 +5701,16 @@
         <v>37.473056</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -5756,11 +5724,11 @@
         <v>27.427821999999999</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E12" s="10"/>
       <c r="G12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -5774,16 +5742,16 @@
         <v>37.223215000000003</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B14">
         <v>-79.024995599999997</v>
@@ -5792,21 +5760,21 @@
         <v>36.001745499999998</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B15" s="10">
         <v>-80.907136899999998</v>
@@ -5815,21 +5783,21 @@
         <v>27.213987700000001</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B16">
         <v>-81.965361400000006</v>
@@ -5838,15 +5806,15 @@
         <v>27.8745254</v>
       </c>
       <c r="E16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" t="s">
         <v>177</v>
-      </c>
-      <c r="G16" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B17" s="10">
         <v>-81.880556400000003</v>
@@ -5855,21 +5823,21 @@
         <v>26.674672000000001</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F17">
         <v>2009</v>
       </c>
       <c r="G17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B18" s="10">
         <v>-80.853750700000006</v>
@@ -5878,21 +5846,21 @@
         <v>27.329125999999999</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B19">
         <v>-80.869715799999994</v>
@@ -5901,21 +5869,21 @@
         <v>27.5020904</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B20">
         <v>-80.398945299999994</v>
@@ -5924,21 +5892,21 @@
         <v>27.592262000000002</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B21">
         <v>-80.399409399999996</v>
@@ -5947,21 +5915,21 @@
         <v>27.602654600000001</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F21">
         <v>2010</v>
       </c>
       <c r="G21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B22" s="10">
         <v>-80.479466200000005</v>
@@ -5970,21 +5938,21 @@
         <v>27.609477500000001</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B23" s="10">
         <v>-81.445307999999997</v>
@@ -5993,21 +5961,21 @@
         <v>28.5647631</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F23">
         <v>2009</v>
       </c>
       <c r="G23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B24" s="10">
         <v>-82.477197000000004</v>
@@ -6016,21 +5984,21 @@
         <v>29.923072999999999</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B25" s="10">
         <v>-85.024425500000007</v>
@@ -6039,21 +6007,21 @@
         <v>34.827157800000002</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B26">
         <v>-76.535835800000001</v>
@@ -6062,21 +6030,21 @@
         <v>39.197844400000001</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B27">
         <v>-76.519799699999993</v>
@@ -6085,21 +6053,21 @@
         <v>39.241779600000001</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F27">
         <v>2015</v>
       </c>
       <c r="G27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B28">
         <v>-76.262986100000006</v>
@@ -6108,21 +6076,21 @@
         <v>39.7560024</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F28">
         <v>2009</v>
       </c>
       <c r="G28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" s="10">
         <v>-73.828925999999996</v>
@@ -6131,21 +6099,21 @@
         <v>40.584173399999997</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B30" s="10">
         <v>3.5740601999999999</v>
@@ -6154,16 +6122,16 @@
         <v>51.082552</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E30" s="10"/>
       <c r="G30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B31" s="10">
         <v>16.430962999999998</v>
@@ -6172,11 +6140,11 @@
         <v>48.197578999999998</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -6190,12 +6158,12 @@
         <v>-19.3</v>
       </c>
       <c r="G32" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B33" s="10">
         <v>-76.900000000000006</v>
@@ -6204,11 +6172,11 @@
         <v>39</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E33" s="10"/>
       <c r="G33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -6222,11 +6190,11 @@
         <v>38.784427000000001</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E34" s="10"/>
       <c r="G34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -6240,10 +6208,10 @@
         <v>39.131529</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G35" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -6257,10 +6225,10 @@
         <v>39.449888999999999</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -6274,11 +6242,11 @@
         <v>38.609043200000002</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E37" s="10"/>
       <c r="G37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -6292,16 +6260,16 @@
         <v>37.247632000000003</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -6315,16 +6283,16 @@
         <v>36.200000000000003</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F39">
         <v>2009</v>
       </c>
       <c r="G39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -6338,16 +6306,16 @@
         <v>36.080810999999997</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E40" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G40" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -6361,16 +6329,16 @@
         <v>29.645575999999998</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E41" s="10"/>
       <c r="G41" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B42" s="10">
         <v>-98.806156999999999</v>
@@ -6379,21 +6347,21 @@
         <v>29.491195399999999</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G42" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B43" s="10">
         <v>16.163287777777775</v>
@@ -6402,16 +6370,16 @@
         <v>51.627626666666664</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E43" s="10"/>
       <c r="G43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B44">
         <v>-103.3499748</v>
@@ -6420,21 +6388,21 @@
         <v>34.178595899999998</v>
       </c>
       <c r="D44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G44" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B45" s="10">
         <v>-75.900000000000006</v>
@@ -6443,11 +6411,11 @@
         <v>39</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E45" s="10"/>
       <c r="G45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -6477,8 +6445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6502,361 +6470,365 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="24" t="s">
-        <v>277</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="F1" s="23" t="s">
+      <c r="A1" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="B2" s="17">
+      <c r="A2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="12">
         <v>15</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="D2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="12">
         <v>365.25</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="16" t="str">
+      <c r="A3" s="5" t="str">
         <f>A2</f>
         <v>ATS productivity (high lat)</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="12">
         <f>B2*$G$2*$G$3/$G$4</f>
         <v>54.787500000000001</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="12">
         <f>100*100</f>
         <v>10000</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" s="17">
+      <c r="A4" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="12">
         <v>25</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="D4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="12">
         <v>1000000</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="12" t="str">
+      <c r="A5" s="5" t="str">
         <f>A4</f>
         <v>ATS productivity (equator)</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <f>B4*$G$2*$G$3/$G$4</f>
         <v>91.3125</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="F5" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="D5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="12">
         <v>1000</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="B6" s="13">
+      <c r="A6" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="12">
         <v>40</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="F6" s="12" t="s">
+      <c r="D6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="12">
         <v>1000000000000000</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="B7" s="13">
+      <c r="A7" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="12">
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="F7" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="D7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G7" s="12">
         <v>1000</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="B8" s="13">
+      <c r="A8" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="12">
         <f>(B5-B3)/(B7-B6)</f>
         <v>-0.91312499999999996</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="F8" t="s">
+      <c r="D8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="12">
         <f>(G9+2*G12)/G9</f>
         <v>3.6641245524935475</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B9" s="12">
+        <v>91</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="12">
+        <v>12.010999999999999</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="13">
-        <v>91</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="13">
-        <v>12.010999999999999</v>
-      </c>
-      <c r="H9" s="12" t="s">
+      <c r="B10" s="12">
+        <v>410</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G10" s="12">
+        <v>1.008</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="B10" s="13">
-        <v>410</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="F10" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="G10" s="13">
-        <v>1.008</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="B11" s="17">
+      <c r="A11" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="12">
         <f>B10*G31</f>
         <v>873300000000</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="F11" s="12" t="s">
+      <c r="D11" s="12"/>
+      <c r="F11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <v>14.007</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" s="13">
+      <c r="A12" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" s="12">
         <v>2</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="D12" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <v>15.9994</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="16" t="s">
-        <v>282</v>
-      </c>
-      <c r="B13" s="17">
+      <c r="A13" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="12">
         <f>B12*G31</f>
         <v>4260000000</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>30.97</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="F14" s="12" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="F14" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="12">
         <f>D38</f>
         <v>0.35830664911296195</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="5" t="s">
         <v>108</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="25" t="s">
-        <v>278</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="A15" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="12">
         <f>D41</f>
         <v>6.3071759492481047E-2</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="5" t="s">
         <v>109</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="B16" s="19">
+      <c r="A16" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16" s="12">
         <v>5</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>287</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="D16" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="12">
         <f>D42</f>
         <v>8.7158759525689748E-3</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="5" t="s">
         <v>110</v>
       </c>
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="12">
         <v>75845109000000</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>288</v>
+      <c r="D17" s="5" t="s">
+        <v>284</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="12">
         <v>0.26417200000000002</v>
       </c>
       <c r="H17" s="5" t="s">
@@ -6866,22 +6838,22 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="B18" s="13">
+      <c r="A18" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="12">
         <v>104.9</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>283</v>
+      <c r="D18" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="12">
         <v>2.47105</v>
       </c>
       <c r="H18" s="5" t="s">
@@ -6890,21 +6862,21 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="16" t="s">
-        <v>190</v>
-      </c>
-      <c r="B19" s="17">
+      <c r="A19" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="12">
         <f>B18*$G$6/$G$4</f>
         <v>104900000000</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="5"/>
       <c r="F19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="12">
         <f>1/G18</f>
         <v>0.40468626697153032</v>
       </c>
@@ -6913,22 +6885,22 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B20" s="13">
+      <c r="A20" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="12">
         <v>8</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>283</v>
+      <c r="D20" s="5" t="s">
+        <v>279</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="12">
         <f>1/2.54</f>
         <v>0.39370078740157477</v>
       </c>
@@ -6937,94 +6909,94 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="B21" s="17">
+      <c r="A21" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="12">
         <f>B20*$G$6/$G$4</f>
         <v>8000000000</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="16"/>
+      <c r="D21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="G21" s="14">
+        <v>182</v>
+      </c>
+      <c r="G21" s="12">
         <v>3.28084</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="12">
         <v>250000</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>260</v>
+      <c r="D22" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="G22" s="14">
+        <v>204</v>
+      </c>
+      <c r="G22" s="12">
         <v>1.3079499999999999</v>
       </c>
-      <c r="H22" s="14" t="s">
-        <v>207</v>
+      <c r="H22" s="12" t="s">
+        <v>205</v>
       </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <v>1000000</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>260</v>
+      <c r="D23" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="12">
         <f>1000000*G24/2000</f>
         <v>1.1023099999999999</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="12" t="s">
         <v>4</v>
       </c>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <v>5</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>260</v>
+      <c r="D24" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="12">
         <f>0.00220462</f>
         <v>2.20462E-3</v>
       </c>
@@ -7034,22 +7006,22 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="12">
         <v>100000</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>260</v>
+      <c r="D25" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="12">
         <v>9.2902999999999998E-6</v>
       </c>
       <c r="H25" s="5" t="s">
@@ -7057,22 +7029,22 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <v>0.05</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>260</v>
+      <c r="D26" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="12">
         <v>5280</v>
       </c>
       <c r="H26" s="5" t="s">
@@ -7080,21 +7052,21 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="12">
         <f>(B$25/B$24)+B22*B$26</f>
         <v>32500</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="12"/>
+      <c r="D27" s="5"/>
       <c r="F27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="12">
         <v>0.453592</v>
       </c>
       <c r="H27" s="5" t="s">
@@ -7103,21 +7075,21 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="12">
         <f>(B$25/B$24)+B23*B$26</f>
         <v>70000</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="12"/>
+      <c r="D28" s="5"/>
       <c r="F28" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="12">
         <v>6.4515999999999998E-4</v>
       </c>
       <c r="H28" s="5" t="s">
@@ -7125,17 +7097,17 @@
       </c>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="13">
+      <c r="A29" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B29" s="12">
         <v>40</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>260</v>
+      <c r="D29" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>14</v>
@@ -7144,72 +7116,72 @@
         <v>1.60934</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="13">
+      <c r="A30" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="12">
         <v>20</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>260</v>
+      <c r="D30" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="G30" s="14">
+        <v>261</v>
+      </c>
+      <c r="G30" s="12">
         <v>1000</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="12">
         <v>0.1</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="G31" s="17">
+      <c r="C31" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="G31" s="12">
         <v>2130000000</v>
       </c>
-      <c r="H31" s="16" t="s">
-        <v>291</v>
+      <c r="H31" s="5" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="B32" s="13">
+      <c r="A32" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" s="12">
         <v>50</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>260</v>
+      <c r="D32" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="12">
         <f>1000/G27</f>
         <v>2204.6244201837776</v>
       </c>
@@ -7218,75 +7190,80 @@
       </c>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B33" s="13">
+      <c r="A33" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" s="12">
         <v>100</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>260</v>
+      <c r="D33" s="5" t="s">
+        <v>256</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="12">
         <f>G32/2000</f>
         <v>1.1023122100918887</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B34" s="13">
+      <c r="A34" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" s="12">
         <v>200</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="G34" s="1">
+      <c r="D34" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="G34" s="12">
         <f>G33*G18</f>
         <v>2.7238685867475616</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="I34" s="22"/>
+      <c r="H34" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="I34" s="14"/>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="G35" s="1"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
+      <c r="A36" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="1"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -7295,51 +7272,54 @@
       <c r="D37" s="5" t="s">
         <v>67</v>
       </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="12">
         <v>106</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="12">
         <f>G9*B38</f>
         <v>1273.1659999999999</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="12">
         <f>C38/C$43</f>
         <v>0.35830664911296195</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="B39" s="14">
+        <v>306</v>
+      </c>
+      <c r="B39" s="12">
         <v>263</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="12">
         <f>G10*B39</f>
         <v>265.10399999999998</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="12">
         <f>C39/C$43</f>
         <v>7.4608123297702472E-2</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B40" s="14">
+        <v>307</v>
+      </c>
+      <c r="B40" s="12">
         <v>110</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="12">
         <f>G12*B40</f>
         <v>1759.934</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="12">
         <f>C40/C$43</f>
         <v>0.49529759214428565</v>
       </c>
@@ -7349,14 +7329,14 @@
       <c r="A41" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="12">
         <v>16</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="12">
         <f>G11*B41</f>
         <v>224.11199999999999</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="12">
         <f>C41/C$43</f>
         <v>6.3071759492481047E-2</v>
       </c>
@@ -7453,10 +7433,10 @@
         <v>21</v>
       </c>
       <c r="R1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
@@ -7499,10 +7479,10 @@
         <v>21</v>
       </c>
       <c r="R2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -7551,7 +7531,7 @@
         <v>26</v>
       </c>
       <c r="R3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S3" s="1">
         <v>53.4</v>
@@ -7606,7 +7586,7 @@
         <v>27</v>
       </c>
       <c r="R4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="S4" s="1">
         <f>'R Variables'!$B$11*Wetlands!S3+'R Variables'!$B$12</f>
@@ -7705,7 +7685,7 @@
         <v>0.35</v>
       </c>
       <c r="T6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -7788,7 +7768,7 @@
         <v>3785.41</v>
       </c>
       <c r="R8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S8" s="1">
         <v>0.4</v>
@@ -7840,7 +7820,7 @@
         <v>0.26</v>
       </c>
       <c r="T9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -7907,7 +7887,7 @@
       </c>
       <c r="L11" s="2"/>
       <c r="R11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S11" s="1">
         <f>S7/Settings!G15</f>
@@ -7919,7 +7899,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="R12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="S12" s="1">
         <f>S10/Settings!$G$16</f>
@@ -7940,47 +7920,47 @@
       </c>
       <c r="L13" s="2"/>
       <c r="R13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="S13" s="1">
         <f>$S$4/S11</f>
         <v>2.7184652379314733</v>
       </c>
       <c r="T13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="R14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="S14" s="1">
         <f>$S$4/S12</f>
         <v>3.5399132100486055</v>
       </c>
       <c r="T14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="R16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="18:20">
       <c r="R17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="18:20">
       <c r="R18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S18" s="1">
         <v>7.3</v>
@@ -7991,7 +7971,7 @@
     </row>
     <row r="19" spans="18:20">
       <c r="R19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="S19" s="1">
         <f>'R Variables'!$B$11*Wetlands!S18+'R Variables'!$B$12</f>
@@ -8003,7 +7983,7 @@
     </row>
     <row r="20" spans="18:20">
       <c r="R20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="S20" s="1">
         <v>25</v>
@@ -8014,7 +7994,7 @@
     </row>
     <row r="21" spans="18:20">
       <c r="R21" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="S21" s="1">
         <f>S20/Settings!G3</f>
@@ -8026,48 +8006,48 @@
     </row>
     <row r="22" spans="18:20">
       <c r="R22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="S22" s="1">
         <v>13</v>
       </c>
       <c r="T22" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="18:20">
       <c r="R23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="S23" s="1">
         <f>S22*Settings!$G$7</f>
         <v>13000</v>
       </c>
       <c r="T23" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="18:20">
       <c r="R24" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S24" s="1">
         <v>1.36</v>
       </c>
       <c r="T24" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="18:20">
       <c r="R25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S25" s="1">
         <f>S24*$S$23</f>
         <v>17680</v>
       </c>
       <c r="T25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="18:20">
@@ -8078,7 +8058,7 @@
         <v>0.19</v>
       </c>
       <c r="T26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="18:20">
@@ -8090,7 +8070,7 @@
         <v>3359.2</v>
       </c>
       <c r="T27" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="18:20">
@@ -8102,7 +8082,7 @@
         <v>1226947.8</v>
       </c>
       <c r="T28" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="18:20">
@@ -8131,7 +8111,7 @@
     </row>
     <row r="31" spans="18:20">
       <c r="R31" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="S31" s="1" t="e">
         <f>S30/Settings!$G$16</f>
@@ -8143,23 +8123,23 @@
     </row>
     <row r="33" spans="18:20">
       <c r="R33" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="18:20">
       <c r="R34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="18:20">
       <c r="R35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="S35" s="1">
         <v>24.8</v>
@@ -8170,7 +8150,7 @@
     </row>
     <row r="36" spans="18:20">
       <c r="R36" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="S36" s="1">
         <f>'R Variables'!$B$11*Wetlands!S35+'R Variables'!$B$12</f>
@@ -8182,7 +8162,7 @@
     </row>
     <row r="37" spans="18:20">
       <c r="R37" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="S37" s="1">
         <v>1.07</v>
@@ -8193,48 +8173,48 @@
     </row>
     <row r="38" spans="18:20">
       <c r="R38" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="S38" s="1">
         <v>4000</v>
       </c>
       <c r="T38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="18:20">
       <c r="R39" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="S39" s="1">
         <f>S38*Settings!$G$7</f>
         <v>4000000</v>
       </c>
       <c r="T39" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="18:20">
       <c r="R40" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S40" s="1">
         <v>1.9</v>
       </c>
       <c r="T40" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="41" spans="18:20">
       <c r="R41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S41" s="1">
         <f>S40*$S$23</f>
         <v>24700</v>
       </c>
       <c r="T41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="18:20">
@@ -8245,7 +8225,7 @@
         <v>0.44</v>
       </c>
       <c r="T42" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="18:20">
@@ -8257,7 +8237,7 @@
         <v>10868</v>
       </c>
       <c r="T43" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="18:20">
@@ -8269,7 +8249,7 @@
         <v>3969537</v>
       </c>
       <c r="T44" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="18:20">
@@ -8298,7 +8278,7 @@
     </row>
     <row r="47" spans="18:20">
       <c r="R47" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="S47" s="1" t="e">
         <f>S46/Settings!$G$16</f>
@@ -8345,7 +8325,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>62</v>
@@ -8354,12 +8334,12 @@
         <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B2" s="1">
         <f>[1]A!$R$66</f>
@@ -8369,24 +8349,24 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B3" s="1">
         <f>'Highway Costs'!B2*Settings!G30*Settings!G29</f>
         <v>14107553603.434601</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B4" s="1">
         <v>12</v>
@@ -8395,24 +8375,24 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B5" s="1">
         <f>B4/Settings!G21</f>
         <v>3.6575998829568039</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B6" s="1">
         <f>B5*B3</f>
@@ -8424,7 +8404,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B7" s="1">
         <f>B6/Settings!G3</f>
@@ -8436,7 +8416,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B8" s="1">
         <f>1000*[2]HF2!$E$67</f>
@@ -8446,12 +8426,12 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B9" s="1">
         <f>1000*[2]HF2!$I$67</f>
@@ -8461,12 +8441,12 @@
         <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B10" s="1">
         <f>B9+B8</f>
@@ -8478,14 +8458,14 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B11" s="1">
         <f>B10/B7</f>
         <v>30400.509579137084</v>
       </c>
       <c r="C11" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:4">

</xml_diff>